<commit_message>
(v2.1.1.9254) fix antimicrobial synonyms
</commit_message>
<xml_diff>
--- a/data-raw/datasets/antimicrobials.xlsx
+++ b/data-raw/datasets/antimicrobials.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>aminacyl,aminopar,aminosalicylate,aminosalicylic,aminosalyl,aminox,apacil,deapasil,entepas,gabbropas,granupas,helipidyl,hellipidyl,nemasol,nippas,osacyl,pamacyl,pamisyl,paramisan,paramycin,parasal,parasalicil,parasalindon,pasade,pasalon,pasara,pascorbic,pasdium,pasem,paser,pasmed,pasnal,pasnodia,pasolac,passodico,pharmakon,propasa,rezipas,salvis,sanipirol,sanipriol,sodiopas,spectrum</t>
+          <t>aminacyl,aminopar,aminosalyl,aminox,apacil,deapasil,entepas,gabbropas,granupas,helipidyl,hellipidyl,nemasol,nippas,osacyl,pamacyl,pamisyl,paramisan,paramycin,parasal,parasalicil,parasalindon,pasade,pasalon,pasara,pascorbic,pasdium,pasem,paser,pasmed,pasnal,pasnodia,pasolac,passodico,pharmakon,propasa,rezipas,salvis,sanipirol,sanipriol,sodiopas,spectrum</t>
         </is>
       </c>
       <c r="J2">
@@ -730,7 +730,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>amicacin,amikacillin,amikacina,amikacine,amikacinum,amikavet,amikin,amikozit,amukin,arikace,briclin,butirosins,kaminax,lukadin,mikavir,potentox,prestwick</t>
+          <t>amikacillin,amikacina,amikacine,amikacinum,amikavet,amikin,amikozit,amukin,arikace,briclin,butirosins,kaminax,lukadin,mikavir,potentox,prestwick</t>
         </is>
       </c>
       <c r="J6" t="e">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>acillin,adobacillin,alpen,amblosin,amcap,amcill,amfipen,ampen,amperil,ampichel,ampicil,ampicilina,ampicillina,ampicilline,ampicillinesalt,ampicillinsalt,ampicillinum,ampicin,ampifarm,ampikel,ampimed,ampinova,ampipenin,ampiscel,ampisyn,ampivax,ampivet,amplacilina,amplin,amplipenyl,amplisom,amplital,austrapen,bayer,binotal,bonapicillin,britacil,campicillin,cimex,citteral,copharcilin,cymbi,delcillin,deripen,divercillin,doktacillin,domicillin,duphacillin,grampenil,guicitrina,guicitrine,lifeampil,marcillin,morepen,norobrittin,nuvapen,omnipen,orbicilina,penbristol,penbritin,penbrock,penialmen,penicillin,penicline,penimic,penizillin,pensyn,pentrex,pentrexl,pentrexyl,pentritin,ponecil,princillin,principen,racenacillin,redicilin,rosampline,roscillin,semicillin,servicillin,sumipanto,supen,synpenin,texcillin,tokiocillin,tolomol,totacillin,totalciclina,totapen,trafarbiot,trifacilina,ukapen,ultrabion,ultrabron,vampen,viccillin,vidocillin,wypicil</t>
+          <t>adobacillin,alpen,amblosin,amcap,amcill,amfipen,ampen,amperil,ampichel,ampicilina,ampicillina,ampicilline,ampicillinesalt,ampicillinsalt,ampicillinum,ampifarm,ampikel,ampimed,ampinova,ampipenin,ampiscel,ampisyn,ampivax,ampivet,amplacilina,amplin,amplipenyl,amplisom,amplital,austrapen,bayer,binotal,bonapicillin,britacil,cimex,citteral,copharcilin,cymbi,delcillin,deripen,divercillin,doktacillin,domicillin,duphacillin,grampenil,guicitrina,guicitrine,lifeampil,marcillin,morepen,norobrittin,nuvapen,omnipen,orbicilina,penbristol,penbritin,penbrock,penialmen,penicline,penimic,penizillin,pensyn,pentrex,pentrexl,pentrexyl,pentritin,ponecil,princillin,principen,racenacillin,redicilin,rosampline,roscillin,semicillin,servicillin,sumipanto,supen,synpenin,texcillin,tokiocillin,tolomol,totacillin,totalciclina,totapen,trafarbiot,trifacilina,ukapen,ultrabion,ultrabron,vampen,viccillin,vidocillin,wypicil</t>
         </is>
       </c>
       <c r="J14">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>aritromicina,aruzilina,azasite,azenil,azifast,azigram,azimakrol,azithramycine,azithrocin,azithromycine,azithromycinum,azitrocin,azitromax,azitromicina,azitromicine,azitromin,aziwin,aziwok,aztrin,azyter,hemomycin,macrozit,misultina,mixoterin,setron,sumamed,tobil,toraseptol,tromix,trozocina,trulimax,xithrone,zentavion,zifin,zithrax,zithromac,zithromax,zithromycin,zitrim,zitromax,zitrotek,zythromax</t>
+          <t>aritromicina,aruzilina,azasite,azenil,azifast,azigram,azimakrol,azithramycine,azithrocin,azithromycine,azithromycinum,azitrocin,azitromax,azitromicina,azitromicine,azitromin,aziwin,aziwok,aztrin,azyter,hemomycin,macrozit,misultina,mixoterin,setron,sumamed,tobil,toraseptol,tromix,trozocina,trulimax,xithrone,zentavion,zifin,zithrax,zithromac,zithromax,zitrim,zitromax,zitrotek,zythromax</t>
         </is>
       </c>
       <c r="J27">
@@ -2444,7 +2444,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>albac,altracin,ayfivin,baciferm,baciguent,baciim,baciliquin,bacilliquin,baciquent,bacitracina,bacitracine,bacitracinum,citracin,fortracin,mycitracin,parentracin,penitracin,septa,topitracin,topitrasin,tropitracin,zutracin</t>
+          <t>albac,altracin,ayfivin,baciferm,baciguent,baciim,baciliquin,bacilliquin,baciquent,bacitracina,bacitracine,bacitracinum,fortracin,mycitracin,parentracin,penitracin,septa,topitracin,topitrasin,tropitracin,zutracin</t>
         </is>
       </c>
       <c r="J34" t="e">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>bencilpenicilina,benzopenicillin,benzylpenicilline,benzylpenicillinum,capicillin,cillora,cilloral,cilopen,cintrisul,cosmopen,cristapen,crystapen,dropcillin,eskacillin,ethacillin,falapen,forpen,galofak,gelacillin,hipercilina,hyasorb,hylenta,lemopen,liquacillin,liquapen,monocillin,monopen,mycofarm,novocillin,penalev,penicillinum,penilaryn,penisem,pentid,pentids,pfizerpen,pharmacillin,pradupen,scotcil,sugracillin,sugracillinsalt,tabilin,ursopen,veticillin</t>
+          <t>bencilpenicilina,benzopenicillin,benzylpenicilline,benzylpenicillinum,capicillin,cillora,cilloral,cilopen,cintrisul,cosmopen,cristapen,crystapen,dropcillin,eskacillin,falapen,forpen,galofak,gelacillin,hipercilina,hyasorb,hylenta,lemopen,liquacillin,liquapen,monocillin,monopen,mycofarm,novocillin,penalev,penicillinum,penilaryn,penisem,pentid,pentids,pfizerpen,pharmacillin,pradupen,scotcil,sugracillin,sugracillinsalt,tabilin,ursopen,veticillin</t>
         </is>
       </c>
       <c r="J39" t="e">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>alenfral,alfacet,alfatil,ceclor,cefachlor,cefaclorum,cefeaclor,cephaclor,cephalexin,compound,distaclor,keflor,kefolor,kefral,keftab,keftid,lilly,lopac,panacef,panoral,raniclor</t>
+          <t>alenfral,alfacet,alfatil,ceclor,cefachlor,cefaclorum,cefeaclor,cephaclor,compound,distaclor,keflor,kefolor,kefral,keftab,keftid,lilly,lopac,panacef,panoral,raniclor</t>
         </is>
       </c>
       <c r="J56">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>adcadina,alcephin,alexin,alsporin,ambal,amplex,aristosporin,azabort,bactopenor,beliam,biocef,carnosporin,cefablan,cefacet,cefadal,cefadin,cefadina,cefalekey,cefaleksin,cefalessina,cefalexgobens,cefalexina,cefalexine,cefalexinum,cefalin,cefalival,cefaloto,cefanex,cefaseptin,cefax,ceffanex,cefibacter,ceflax,ceforal,cefovit,celexin,cepastar,cepexin,cephacillin,cephalexine,cephalexinum,cephalobene,cephanasten,cephaxin,cephin,cepol,ceporex,ceporexin,ceporexine,cerexin,cerexins,check,cophalexin,domucef,doriman,durantel,efemida,erocetin,factagard,felexin,fexin,ibilex,ibrexin,inphalex,karilexina,kefalospes,keflet,keflex,kefolan,keforal,kekrinal,kidolex,lafarine,larixin,lenocef,lexibiotico,loisine,lonflex,lopilexin,losporal,madlexin,maksipor,mamalexin,mamlexin,medolexin,medoxine,neokef,neolexina,noveol,novolexin,nufex,optocef,oracef,oriphex,oroxin,ortisporina,ospexin,palitrex,panixine,pectril,prindex,pyassan,rilexine,roceph,rogevil,sanaxin,sartosona,sencephalin,sepexin,servicef,servispor,sialexin,sinthecillin,sintolexyn,sporicef,sporidex,syncl,syncle,synecl,taicelexin,tepaxin,theratrex,tokiolexin,uphalexin,viosporine,voxxim,winlex,zabytrex,zozarine</t>
+          <t>adcadina,alcephin,alsporin,ambal,amplex,aristosporin,azabort,bactopenor,beliam,biocef,carnosporin,cefablan,cefacet,cefadal,cefadin,cefadina,cefalekey,cefaleksin,cefalessina,cefalexgobens,cefalexina,cefalexine,cefalexinum,cefalin,cefalival,cefaloto,cefanex,cefaseptin,cefax,ceffanex,cefibacter,ceflax,ceforal,cefovit,celexin,cepastar,cepexin,cephacillin,cephalexine,cephalexinum,cephalobene,cephanasten,cephaxin,cephin,cepol,ceporex,ceporexin,ceporexine,cerexin,cerexins,check,cophalexin,domucef,doriman,durantel,efemida,erocetin,factagard,felexin,fexin,ibilex,ibrexin,inphalex,karilexina,kefalospes,keflet,keflex,kefolan,keforal,kekrinal,kidolex,lafarine,larixin,lenocef,lexibiotico,loisine,lonflex,lopilexin,losporal,madlexin,maksipor,mamalexin,mamlexin,medolexin,medoxine,neokef,neolexina,noveol,novolexin,nufex,optocef,oracef,oriphex,oroxin,ortisporina,ospexin,palitrex,panixine,pectril,prindex,pyassan,rilexine,roceph,rogevil,sanaxin,sartosona,sencephalin,sepexin,servicef,servispor,sialexin,sinthecillin,sintolexyn,sporicef,sporidex,syncl,syncle,synecl,taicelexin,tepaxin,theratrex,tokiolexin,uphalexin,viosporine,voxxim,winlex,zabytrex,zozarine</t>
         </is>
       </c>
       <c r="J58">
@@ -3982,7 +3982,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>aliporina,ampligram,cefaloridin,cefaloridina,cefaloridinum,cefalorizin,ceflorin,cepaloridin,cepalorin,cephalomycine,cephaloridin,cephaloridine,cephaloridinum,ceporan,ceporin,ceporine,cilifor,deflorin,faredina,floridin,glaxoridin,intrasporin,keflodin,keflordin,kefloridin,kefspor,lloncefal,loridine,sasperin,sefacin,verolgin,vioviantine</t>
+          <t>aliporina,ampligram,cefaloridin,cefaloridina,cefaloridinum,cefalorizin,ceflorin,cepaloridin,cepalorin,cephalomycine,cephaloridin,cephaloridine,cephaloridinum,ceporan,ceporin,ceporine,cilifor,deflorin,faredina,floridin,glaxoridin,intrasporin,keflodin,keflordin,kefloridin,kefspor,lloncefal,sasperin,sefacin,verolgin,vioviantine</t>
         </is>
       </c>
       <c r="J59" t="e">
@@ -4366,7 +4366,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>ancef,atirin,biazolina,cefabiozim,cefacidal,cefalomicina,cefamedin,cefamezin,cefazil,cefazina,cefazolina,cefazoline,cefazolinsalt,cefazolinum,cephamezine,cephazolidin,cephazolin,cephazoline,elzogram,firmacef,gramaxin,kefzol,lampocef,liviclina,neofazol,oprea,recef,totacef,zolicef,zolin,zolisint</t>
+          <t>ancef,atirin,biazolina,cefabiozim,cefacidal,cefalomicina,cefamedin,cefamezin,cefazil,cefazina,cefazolina,cefazoline,cefazolinsalt,cefazolinum,cephamezine,cephazolidin,cephazolin,cephazoline,elzogram,firmacef,gramaxin,kefzol,lampocef,liviclina,neofazol,oprea,recef,totacef,zolicef,zolisint</t>
         </is>
       </c>
       <c r="J65" t="e">
@@ -6200,7 +6200,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>anticefotaxime,cefotax,cefotaxim,cefotaxima,cefotaximesalt,cefotaximsalt,cefotaximum,cephotaxim,cephotaxime,claforan,kefotex,omnatax,pretor,ralopar,taxim,tolycar,tolycor,zariviz</t>
+          <t>anticefotaxime,cefotax,cefotaxim,cefotaxima,cefotaximesalt,cefotaximsalt,cefotaximum,cephotaxim,cephotaxime,claforan,kefotex,omnatax,pretor,ralopar,tolycar,tolycor,zariviz</t>
         </is>
       </c>
       <c r="J95" t="e">
@@ -6924,7 +6924,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>cefpiramida,cefpiramidesalt,cefpiramido,cefpiramidum,sepatren,suncefal,tamicin</t>
+          <t>cefpiramida,cefpiramidesalt,cefpiramido,cefpiramidum,sepatren,suncefal</t>
         </is>
       </c>
       <c r="J107" t="e">
@@ -7658,7 +7658,7 @@
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>ceftazimide,ceptaz,fortam,fortaz,fortum,glazidim,kefazim,modacin,pentacef,tazicef,tazidime,tizime,zidim</t>
+          <t>ceftazimide,ceptaz,fortam,fortaz,fortum,glazidim,kefazim,modacin,pentacef,tazicef,tizime</t>
         </is>
       </c>
       <c r="J119" t="e">
@@ -8646,7 +8646,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>bioracef,ceftin,cefurax,cefuroximaxetil,celocid,cepazine,cethixim,cetoxil,coliofossim,curocef,elobact,furoxime,kalcef,maxitil,medoxm,nivador,novador,novocef,oraxim,zinat,zoref</t>
+          <t>bioracef,ceftin,cefurax,cefuroximaxetil,celocid,cepazine,cethixim,cetoxil,coliofossim,curocef,elobact,kalcef,maxitil,medoxm,nivador,novador,novocef,oraxim,zinat,zoref</t>
         </is>
       </c>
       <c r="J135" t="e">
@@ -8952,7 +8952,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>alficetyn,ambofen,amphenicol,amphicol,amseclor,anacetin,aquamycetin,austracil,austracol,biocetin,biophenicol,catilan,chemicetin,chemicetina,chlomin,chlomycol,chloramex,chloramfenikol,chloramficin,chloramfilin,chloramphenicole,chloramphenicolum,chloramsaar,chlorasol,chlorbiotic,chloricol,chlornitromycin,chloroamphenicol,chlorocaps,chlorocid,chlorocide,chlorocin,chlorocol,chlorofair,chloromax,chloromycetin,chloromycetny,chloromyxin,chloronitrin,chloroptic,chlorovules,cidocetine,ciplamycetin,cloramfen,cloramfenicol,cloramfenicolo,cloramficin,cloramicol,cloramidina,cloranfenicol,cloroamfenicolo,clorocyn,cloromisan,clorosintex,comycetin,cylphenicol,desphen,detreomycin,detreomycine,dextramycin,dextromycetin,doctamicina,econochlor,embacetin,emetren,enicol,enteromycetin,erbaplast,ertilen,farmicetina,fenicol,globenicol,glorous,gloveticol,halcetin,halomycetin,hortfenicol,intramycetin,isicetin,ismicetina,isophenicol,juvamycetin,kamaver,kemicetina,kemicetine,kloramfenikol,klorita,laevomycetinum,leukamycin,leukomyan,leukomycin,levocin,levomicetina,levomitsetin,levomycetin,levoplast,levosin,levovetin,loromisan,loromisin,mastiphen,maybridge,mediamycetine,medichol,micloretin,micochlorine,micoclorina,microcetina,mychel,mycinol,myclocin,mycochlorin,novochlorocap,novomycetin,novophenicol,ocuphenicol,oftalent,oleomycetin,opclor,opelor,ophthochlor,ophthocort,ophtochlor,optomycin,otachron,otophen,pantovernil,paraxin,pentamycetin,petnamycetin,quemicetina,rivomycin,romphenil,ronphenil,septicol,sificetina,sintomicetin,sintomicetina,soluthor,stanomycetin,synthomycetin,synthomycetine,synthomycine,syntomycin,tevcocin,tevcosin,tifomycin,tifomycine,tiromycetin,treomicetina,tyfomycine,unimycetin,veticol,viceton</t>
+          <t>alficetyn,ambofen,amphicol,amseclor,anacetin,aquamycetin,austracil,austracol,biocetin,biophenicol,catilan,chemicetin,chemicetina,chlomin,chlomycol,chloramex,chloramfenikol,chloramficin,chloramfilin,chloramphenicole,chloramphenicolum,chloramsaar,chlorasol,chlorbiotic,chloricol,chlornitromycin,chloroamphenicol,chlorocaps,chlorocid,chlorocide,chlorocin,chlorocol,chlorofair,chloromax,chloromycetin,chloromycetny,chloromyxin,chloronitrin,chloroptic,chlorovules,cidocetine,ciplamycetin,cloramfen,cloramfenicol,cloramfenicolo,cloramficin,cloramicol,cloramidina,cloranfenicol,cloroamfenicolo,clorocyn,cloromisan,clorosintex,comycetin,cylphenicol,desphen,detreomycin,detreomycine,dextramycin,dextromycetin,doctamicina,econochlor,embacetin,emetren,enteromycetin,erbaplast,ertilen,farmicetina,globenicol,glorous,gloveticol,halcetin,halomycetin,hortfenicol,intramycetin,isicetin,ismicetina,isophenicol,juvamycetin,kamaver,kemicetina,kemicetine,kloramfenikol,klorita,laevomycetinum,leukamycin,leukomyan,leukomycin,levocin,levomicetina,levomitsetin,levomycetin,levoplast,levosin,levovetin,loromisan,loromisin,mastiphen,maybridge,mediamycetine,medichol,micloretin,micochlorine,micoclorina,microcetina,mychel,mycinol,myclocin,mycochlorin,novochlorocap,novomycetin,novophenicol,ocuphenicol,oftalent,oleomycetin,opclor,opelor,ophthochlor,ophthocort,ophtochlor,optomycin,otachron,otophen,pantovernil,paraxin,pentamycetin,petnamycetin,quemicetina,rivomycin,romphenil,ronphenil,septicol,sificetina,sintomicetin,sintomicetina,soluthor,stanomycetin,synthomycetin,synthomycetine,synthomycine,syntomycin,tevcocin,tevcosin,tifomycin,tifomycine,tiromycetin,treomicetina,tyfomycine,unimycetin,veticol,viceton</t>
         </is>
       </c>
       <c r="J140">
@@ -9018,7 +9018,7 @@
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>acronize,alexomycin,aueromycin,aureocarmyl,aureociclina,aureocina,aureocycline,aureomycin,aureomykoin,aurofac,auxeomycin,biomitsin,biomycin,chlormax,chlorotetracycline,chlortetracyclinum,chrysomykine,clorocipan,clortetraciclina,clortetrin,declomycin,declostatin,deganol,demeclor,demeplus,demetraciclina,demetraclin,detracin,detravis,diuciclin,duomycin,elkamicina,flamycin,isphamycin,ledermicina,ledermycin,ledermycine,mexocine,novotriclina,pennchlor,perciclina,periciclina,sumaclina,tetra,uromycin,veraciclina</t>
+          <t>acronize,alexomycin,aueromycin,aureocarmyl,aureociclina,aureocina,aureocycline,aureomycin,aureomykoin,aurofac,auxeomycin,biomitsin,biomycin,chlormax,chlorotetracycline,chlortetracyclinum,chrysomykine,clorocipan,clortetraciclina,clortetrin,declomycin,declostatin,deganol,demeclor,demeplus,demetraciclina,demetraclin,detracin,detravis,diuciclin,duomycin,elkamicina,flamycin,isphamycin,ledermicina,ledermycin,ledermycine,mexocine,novotriclina,pennchlor,perciclina,periciclina,sumaclina,uromycin,veraciclina</t>
         </is>
       </c>
       <c r="J141">
@@ -9266,7 +9266,7 @@
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>alcipro,bacquinor,baflox,belmacina,bernoflox,catex,cenin,ceprimax,cetraxal,ciflan,ciflosin,ciflox,cifloxin,cilab,cilox,ciloxan,cipad,ciplus,ciprecu,ciprenit,ciprine,ciprinol,cipro,ciprobay,ciprocinal,ciprocinol,ciprodar,ciproflox,ciprofloxacina,ciprofloxacine,ciprofloxacino,ciprofloxacinum,ciprofur,ciprogis,ciproktan,ciprolin,ciprolon,cipromycin,cipronex,ciprooxacin,cipropol,ciproquinol,ciprowin,ciproxan,ciproxin,ciproxina,ciproxine,ciriax,citeral,citopcin,cixan,corsacin,cunesin,cycin,cyprobay,cyproxan,disfabac,felixene,fimoflox,flociprin,floxacipron,flunas,globuce,inkamil,ipiflox,italnik,keefloxin,linhaliq,loxacid,loxan,lypro,megaflox,microgan,nixin,novidat,novoquin,ofitin,oftacilox,ophaflox,otiprio,phaproxin,piprol,plenolyt,probiox,proflaxin,proksi,proquin,proxacin,quinoflox,quinolid,quintor,quipro,rancif,renator,roflazin,roxytal,sepcen,septicide,septocipro,siprogut,sophixin,spitacin,strox,suiflox,superocin,supraflox,uritent,utiminx,velmonit,zumaflox</t>
+          <t>alcipro,bacquinor,baflox,belmacina,bernoflox,catex,cenin,ceprimax,cetraxal,ciflan,ciflosin,cifloxin,cilab,cilox,ciloxan,cipad,ciplus,ciprecu,ciprenit,ciprine,ciprinol,cipro,ciprobay,ciprocinal,ciprocinol,ciprodar,ciproflox,ciprofloxacina,ciprofloxacine,ciprofloxacino,ciprofloxacinum,ciprofur,ciprogis,ciproktan,ciprolin,ciprolon,cipromycin,cipronex,ciprooxacin,cipropol,ciproquinol,ciprowin,ciproxan,ciproxin,ciproxina,ciproxine,ciriax,citeral,citopcin,cixan,corsacin,cunesin,cycin,cyprobay,cyproxan,disfabac,felixene,fimoflox,flociprin,floxacipron,flunas,globuce,inkamil,ipiflox,italnik,keefloxin,linhaliq,loxacid,loxan,lypro,megaflox,microgan,nixin,novidat,novoquin,ofitin,oftacilox,ophaflox,otiprio,phaproxin,piprol,plenolyt,probiox,proflaxin,proksi,proquin,proxacin,quinoflox,quinolid,quintor,quipro,rancif,renator,roflazin,roxytal,sepcen,septicide,septocipro,siprogut,sophixin,spitacin,strox,suiflox,superocin,supraflox,uritent,utiminx,velmonit,zumaflox</t>
         </is>
       </c>
       <c r="J145">
@@ -9518,7 +9518,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>abbotic,abboticine,astromen,biaxin,bicrolid,bristamycin,clacee,clacid,clacine,clambiotic,clarem,claribid,claricide,claridar,claripen,clarith,clarithromycine,clarithromycinum,claritromicina,clarosip,clathromycin,crixan,cyllid,cyllind,eratrex,esinol,ethril,fromilid,gallimycin,helas,heliclar,klabax,klacid,klaciped,klaricid,klarid,klarin,kofron,mabicrol,macladin,maclar,mavid,meberyt,pediamycin,qidmycin,veclam,wyamycin,zeclar</t>
+          <t>abbotic,abboticine,astromen,biaxin,bicrolid,bristamycin,clacee,clacid,clacine,clambiotic,clarem,claribid,claricide,claridar,claripen,clarith,clarithromycine,clarithromycinum,claritromicina,clarosip,clathromycin,crixan,cyllid,cyllind,eratrex,esinol,fromilid,gallimycin,helas,heliclar,klabax,klacid,klaciped,klaricid,klarid,klarin,kofron,mabicrol,macladin,maclar,mavid,meberyt,pediamycin,qidmycin,veclam,wyamycin,zeclar</t>
         </is>
       </c>
       <c r="J149">
@@ -10074,7 +10074,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>alevazol,bisphenyl,canesten,canestene,canestine,canifug,chlotrimazole,clomatin,clotrimaderm,clotrimazol,clotrimazolum,coltrimazole,cutistad,diphenylmethane,empecid,esparol,femmesil,footlogix,fortinia,gynix,imidazole,jidesheng,klotrimazole,lakesia,lombazol,lombazole,lombazolum,lotrimax,lotrimin,monobaycuten,mycelax,mycelex,mycofug,mycosporin,mykosporin,nalbix,otomax,pedesil,pedisafe,rimazole,ringworm,stiemazol,tibatin,trimysten,trivagizole</t>
+          <t>alevazol,bisphenyl,canesten,canestene,canestine,canifug,chlotrimazole,clomatin,clotrimaderm,clotrimazol,clotrimazolum,coltrimazole,cutistad,diphenylmethane,empecid,esparol,femmesil,footlogix,fortinia,gynix,imidazole,jidesheng,klotrimazole,lakesia,lombazol,lombazole,lombazolum,lotrimax,lotrimin,monobaycuten,mycelax,mycelex,mycofug,mycosporin,mykosporin,nalbix,otomax,pedesil,pedisafe,ringworm,stiemazol,tibatin,trimysten,trivagizole</t>
         </is>
       </c>
       <c r="J158" t="e">
@@ -10136,7 +10136,7 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>ankerbin,austrastaph,biocloxin,brispen,chloroxacillin,ciclex,clocil,clossacillina,cloxacilina,cloxacillinanhydrous,cloxacilline,cloxacillinsalt,cloxacillinum,cloxapen,constaphyl,dariclox,dichlorstapenor,diclocil,dicloxacillinhydrate,diflor,digloxilline,dycill,dynapen,ekvacillin,gelstaph,novapen,noxaben,orbenin,pathocil,stampen,staphybiotic,syntarpen,syntarpensalt,tegopen</t>
+          <t>ankerbin,austrastaph,biocloxin,brispen,chloroxacillin,ciclex,clocil,clossacillina,cloxacilina,cloxacillinanhydrous,cloxacilline,cloxacillinsalt,cloxacillinum,cloxapen,constaphyl,dariclox,dichlorstapenor,diclocil,dicloxacillinhydrate,diflor,digloxilline,dynapen,ekvacillin,gelstaph,novapen,noxaben,orbenin,pathocil,stampen,staphybiotic,syntarpen,syntarpensalt,tegopen</t>
         </is>
       </c>
       <c r="J159">
@@ -10326,7 +10326,7 @@
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>cicloserina,closerin,closina,cyclorin,cycloserin,cycloserinum,farmiserina,levcicloserina,levcycloserine,levcycloserinum,micoserina,miroserina,miroseryn,novoserin,oxamicina,oxamycin,seromycin,tebemicina,tisomycin,wasserina</t>
+          <t>cicloserina,closina,cyclorin,cycloserin,cycloserinum,farmiserina,levcicloserina,levcycloserine,levcycloserinum,micoserina,miroserina,miroseryn,novoserin,oxamicina,oxamycin,seromycin,tebemicina,wasserina</t>
         </is>
       </c>
       <c r="J162">
@@ -11146,7 +11146,7 @@
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>abbocin,alamycin,aquacycline,biosolvomycin,biotet,bisolvomycin,chrysocin,dalimycin,dalinmycin,deoxymykoin,dossiciclina,doxiciclina,doxirobe,doxitard,doxivetin,doxycen,doxychel,doxycin,doxycyclin,doxycyclinum,doxylin,doxysol,doxytetracycline,elinton,engemycin,hydrocyclin,imperacin,intaloxin,investin,jenacyclin,liquachel,liviatin,macodyn,mepatar,microdox,mondoxyne,monodox,morgidox,ocudox,okebo,oracea,otetryn,oxacycline,oxamycen,oxatet,oxlopar,oxybiocycline,oxycycline,oxydon,oxyject,oxymykoin,oxysteclin,oxytet,oxytetral,oxytetrin,oxytracyl,oxyvet,stecsolin,supracyclin,terraject,terramycin,toxinal,unimycin,vendarcin,vibramycin,vibramycine,vivox,zenavod</t>
+          <t>abbocin,alamycin,aquacycline,biosolvomycin,biotet,bisolvomycin,chrysocin,dalimycin,dalinmycin,deoxymykoin,dossiciclina,doxiciclina,doxirobe,doxitard,doxivetin,doxycen,doxychel,doxycin,doxycyclin,doxycyclinum,doxylin,doxysol,doxytetracycline,elinton,engemycin,hydrocyclin,imperacin,intaloxin,investin,jenacyclin,liquachel,liviatin,macodyn,mepatar,microdox,mondoxyne,monodox,morgidox,ocudox,okebo,oracea,otetryn,oxacycline,oxamycen,oxatet,oxlopar,oxybiocycline,oxydon,oxyject,oxymykoin,oxysteclin,oxytet,oxytetral,oxytetrin,oxytracyl,oxyvet,stecsolin,supracyclin,terraject,terramycin,toxinal,unimycin,vendarcin,vibramycin,vibramycine,vivox,zenavod</t>
         </is>
       </c>
       <c r="J175">
@@ -11212,7 +11212,7 @@
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>bromazil,chloramizol,clinafarm,deccosil,deccozil,econazol,econazolum,ecostatin,ekonazole,enilconazol,enilconazole,eniloconazol,fecundal,florasan,freshgard,freshguard,fungaflor,fungazil,imaverol,imaversol,imazalil,magnate,spectazole</t>
+          <t>bromazil,chloramizol,clinafarm,deccosil,deccozil,econazolum,ecostatin,ekonazole,enilconazol,enilconazole,eniloconazol,fecundal,florasan,freshgard,freshguard,fungaflor,fungazil,imaverol,imaversol,imazalil,magnate,spectazole</t>
         </is>
       </c>
       <c r="J176" t="e">
@@ -11824,7 +11824,7 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>abboticin,abomacetin,acneryne,acnesol,aknemycin,aknin,benzamycin,derimer,deripil,dotycin,dumotrycin,emgel,emuvin,emycin,endoeritrin,erecin,erisone,eritomicina,eritrocina,eritromicina,ermycin,eryacne,eryacnen,erycen,erycette,erycin,erycinum,eryderm,erydermer,erygel,eryhexal,erymax,erymed,erysafe,erytab,erythro,erythroderm,erythrogran,erythroguent,erythromast,erythromid,erythromycine,erythromycinum,erytop,erytrociclin,ilocaps,ilosone,iloticina,ilotycin,inderm,latotryd,lederpax,mephamycin,mercina,oftamolets,pantoderm,pantodrin,pantomicina,pharyngocin,primacine,propiocine,proterytrin,retcin,robimycin,romycin,sansac,spotex,staticin,stiemicyn,stiemycin,tiprocin,torlamicina,wemid</t>
+          <t>abboticin,abomacetin,acneryne,acnesol,aknemycin,aknin,benzamycin,derimer,deripil,dotycin,dumotrycin,emgel,emuvin,emycin,endoeritrin,erecin,erisone,eritomicina,eritrocina,eritromicina,ermycin,eryacne,eryacnen,erycen,erycette,erycinum,eryderm,erydermer,erygel,eryhexal,erymax,erymed,erysafe,erytab,erythro,erythroderm,erythrogran,erythroguent,erythromast,erythromid,erythromycine,erythromycinum,erytop,erytrociclin,ilocaps,ilosone,iloticina,ilotycin,inderm,latotryd,lederpax,mephamycin,mercina,oftamolets,pantoderm,pantodrin,pantomicina,pharyngocin,primacine,propiocine,proterytrin,retcin,robimycin,sansac,spotex,staticin,stiemicyn,stiemycin,tiprocin,torlamicina,wemid</t>
         </is>
       </c>
       <c r="J186">
@@ -12686,7 +12686,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>alflucoz,alkanazole,baten,biocanol,biozole,biozolene,canzol,cryptal,diflazon,diflucan,dimycon,elazor,flucazol,fluconazol,fluconazoli,fluconazolum,flucoral,flucostat,flukezol,flunazol,flunizol,fluzon,forcan,fuconal,fungata,loitin,mutum,oxifugol,pritenzol,syscan,trican,triconal,triflucan,zemyc,zoltec,zonal</t>
+          <t>alflucoz,alkanazole,baten,biocanol,biozole,biozolene,canzol,cryptal,diflazon,diflucan,dimycon,elazor,flucazol,fluconazoli,fluconazolum,flucoral,flucostat,flukezol,flunazol,flunizol,fluzon,forcan,fuconal,fungata,loitin,mutum,oxifugol,pritenzol,syscan,trican,triconal,triflucan,zemyc,zoltec,zonal</t>
         </is>
       </c>
       <c r="J200">
@@ -13246,7 +13246,7 @@
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>bifuron,corizium,coryzium,diafuron,enterotoxon,furall,furanzolidone,furaxon,furaxone,furazol,furazolidine,furazolidon,furazolidona,furazolidonum,furazolum,furazon,furidon,furmethoxadone,furovag,furox,furoxal,furoxane,furoxon,furoxone,furozolidine,giardil,giarlam,medaron,neftin,nicolen,nifulidone,nifuran,nifurazolidone,nifurazolidonum,nitrofuradoxon,nitrofurazolidone,nitrofurazolidonum,nitrofuroxon,optazol,ortazol,puradin,roptazol,sclaventerol,tikofuran,topazone,trichofuron,tricofuron,tricoron,trifurox,viofuragyn</t>
+          <t>bifuron,corizium,coryzium,diafuron,enterotoxon,furall,furanzolidone,furaxon,furaxone,furazolidine,furazolidon,furazolidona,furazolidonum,furazolum,furidon,furmethoxadone,furovag,furoxal,furoxane,furoxon,furoxone,furozolidine,giardil,giarlam,medaron,neftin,nicolen,nifulidone,nifuran,nifurazolidone,nifurazolidonum,nitrofuradoxon,nitrofurazolidone,nitrofurazolidonum,nitrofuroxon,optazol,ortazol,puradin,roptazol,sclaventerol,tikofuran,topazone,trichofuron,tricofuron,tricoron,trifurox,viofuragyn</t>
         </is>
       </c>
       <c r="J209" t="e">
@@ -13308,7 +13308,7 @@
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>flucidin,fucidate,fucidina,fucidine,fucithalmic,fusidate,fusidicacid,fusidin,fusidine,ramycin,taksta</t>
+          <t>flucidin,fucidate,fucidina,fucidine,fucithalmic,fusidate,fusidicacid,fusidin,fusidine,taksta</t>
         </is>
       </c>
       <c r="J210">
@@ -14656,7 +14656,7 @@
       </c>
       <c r="I232" t="inlineStr">
         <is>
-          <t>abdizide,acetylisoniazide,andrazide,anidrasona,antimicina,antituberkulosum,armacide,armazid,armazide,atcotibine,azuren,cedin,cemidon,chemiazid,chemidon,continazine,cortinazine,cotinazin,cotinizin,defonin,dianicotyl,dibutin,diforin,dinacrin,dinocrin,ditubin,ebidene,eralon,ertuban,eutizon,evalon,fetefu,fimalene,hidranizil,hidrasonil,hidrulta,hidrun,hycozid,hydra,hydrazid,hyozid,hyzyd,idrazil,inizid,ipcazide,iscotin,isidrina,ismazide,isobicina,isocid,isocidene,isocotin,isohydrazide,isokin,isolyn,isonerit,isonex,isoniacid,isoniazida,isoniazide,isoniazidum,isonicazide,isonicid,isonico,isonicotan,isonicotil,isonicotinhydrazid,isonicotinohydrazide,isonide,isonidrin,isonikazid,isonilex,isonin,isonindon,isonirit,isoniton,isonizida,isonizide,isotamine,isotebe,isotebezid,isotinyl,isozid,isozide,isozyd,laniazid,laniozid,mayambutol,mybasan,neoteben,neoxin,neumandin,nevin,niadrin,nicazide,nicetal,nicizina,niconyl,nicotibina,nicotibine,nicotisan,nicozide,nidaton,nidrazid,nikozid,niplen,nitadon,niteban,nitebannsc,nydrazid,nyscozid,pelazid,percin,phthisen,preparation,pycazide,pyreazid,pyricidin,pyridicin,pyrizidin,raumanon,razide,retozide,rifater,rimicid,rimifon,rimiphone,rimitsid,robiselin,robisellin,roxifen,sanohidrazina,sauterazid,sauterzid,soniazid,stanozide,tebecid,tebenic,tebexin,tebilon,tebos,teebaconin,tekazin,tibazide,tibemid,tibiazide,tibinide,tibison,tibivis,tibizide,tibusan,tisin,tisiodrazida,tizide,tubazid,tubazide,tubeco,tubecotubercid,tuberian,tubicon,tubilysin,tubizid,tubomel,tyvid,unicocyde,unicozyde,vazadrine,vederon,zidafimia,zinadon,zonazide</t>
+          <t>abdizide,acetylisoniazide,andrazide,anidrasona,antimicina,antituberkulosum,armacide,armazid,armazide,atcotibine,azuren,cedin,cemidon,chemiazid,chemidon,continazine,cortinazine,cotinazin,cotinizin,defonin,dianicotyl,dibutin,diforin,dinacrin,dinocrin,ditubin,ebidene,eralon,ertuban,eutizon,evalon,fetefu,fimalene,hidranizil,hidrasonil,hidrulta,hidrun,hycozid,hydra,hydrazid,hyozid,hyzyd,idrazil,inizid,ipcazide,iscotin,isidrina,ismazide,isobicina,isocid,isocidene,isocotin,isohydrazide,isokin,isolyn,isonerit,isonex,isoniacid,isoniazida,isoniazide,isoniazidum,isonicazide,isonicid,isonico,isonicotan,isonicotil,isonicotinhydrazid,isonicotinohydrazide,isonide,isonidrin,isonikazid,isonilex,isonin,isonindon,isonirit,isoniton,isonizida,isonizide,isotamine,isotebe,isotebezid,isotinyl,isozid,isozide,isozyd,laniazid,laniozid,mayambutol,mybasan,neoteben,neoxin,neumandin,nevin,niadrin,nicazide,nicetal,nicizina,niconyl,nicotibina,nicotibine,nicotisan,nicozide,nidaton,nidrazid,nikozid,niplen,nitadon,niteban,nitebannsc,nydrazid,nyscozid,pelazid,percin,phthisen,preparation,pycazide,pyreazid,pyricidin,pyridicin,pyrizidin,raumanon,razide,retozide,rifater,rimicid,rimifon,rimiphone,rimitsid,robiselin,robisellin,roxifen,sanohidrazina,sauterazid,sauterzid,stanozide,tebecid,tebenic,tebexin,tebilon,tebos,teebaconin,tekazin,tibazide,tibemid,tibiazide,tibinide,tibison,tibivis,tibizide,tibusan,tisin,tisiodrazida,tizide,tubazid,tubazide,tubeco,tubecotubercid,tuberian,tubicon,tubilysin,tubizid,tubomel,tyvid,unicocyde,unicozyde,vazadrine,vederon,zidafimia,zinadon,zonazide</t>
         </is>
       </c>
       <c r="J232">
@@ -14784,7 +14784,7 @@
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>candistat,canditral,cladosal,fungitraxx,intraconazole,itrac,itraconazol,itraconazolo,itraconazolum,itraconzaole,itrafungol,itralek,itrizole,lozanoc,onmel,oriconazole,sempera,sporamelt,sporanox,sporonox,traconal,triasporin</t>
+          <t>candistat,canditral,cladosal,fungitraxx,intraconazole,itraconazol,itraconazolo,itraconazolum,itraconzaole,itrafungol,itralek,itrizole,lozanoc,onmel,sempera,sporamelt,sporanox,sporonox,traconal,triasporin</t>
         </is>
       </c>
       <c r="J234">
@@ -15520,7 +15520,7 @@
       </c>
       <c r="I246" t="inlineStr">
         <is>
-          <t>aeroquin,cravit,dextrofloxacin,dynaquin,elequine,floxacin,iquix,levaquin,levofiexacin,levofloxacine,levofloxacino,levofloxacinum,loxof,ofloxcacin,oftaquix,quinsair,quixin,tavanic,unibiotic,venaxan</t>
+          <t>aeroquin,cravit,dextrofloxacin,dynaquin,elequine,iquix,levaquin,levofiexacin,levofloxacine,levofloxacino,levofloxacinum,loxof,ofloxcacin,oftaquix,quinsair,quixin,tavanic,unibiotic,venaxan</t>
         </is>
       </c>
       <c r="J246">
@@ -16148,7 +16148,7 @@
       </c>
       <c r="I256" t="inlineStr">
         <is>
-          <t>amygdalate,mandelsaeure,methyl,paramandelate,phenylglycolate,phenylhydroxyacetate,uromaline</t>
+          <t>amygdalate,mandelsaeure,paramandelate,phenylglycolate,phenylhydroxyacetate,uromaline</t>
         </is>
       </c>
       <c r="J256">
@@ -17068,7 +17068,7 @@
       </c>
       <c r="I271" t="inlineStr">
         <is>
-          <t>acromona,anagiardil,arilin,atrivyl,bexon,clont,danizol,deflamon,donnan,efloran,elyzol,entizol,eumin,flagemona,flagesol,flagil,flagyl,flazol,flegyl,florazole,fossyol,giatricol,gineflavir,givagil,hydroxydimetridazole,hydroxymetronidazole,izoklion,klion,klont,mepagyl,meronidal,methronidazole,metric,metrolag,metrolyl,metromidol,metronidaz,metronidazol,metronidazolo,metronidazolum,metroplex,metrotop,mexibol,monagyl,monasin,nalox,nidagyl,noritate,novonidazol,nuvessa,orvagil,polibiotic,protostat,rathimed,rosaced,rosased,sanatrichom,satric,takimetol,trichazol,trichex,trichobrol,trichocide,trichomol,trichopal,trichopol,tricocet,tricom,trikacide,trikamon,trikhopol,trikojol,trikozol,trimeks,trivazol,vagilen,vagimid,vandazole,vertisal,wagitran,zadstat,zidoval</t>
+          <t>acromona,anagiardil,arilin,atrivyl,bexon,clont,danizol,deflamon,donnan,efloran,elyzol,entizol,eumin,flagemona,flagesol,flagil,flagyl,flazol,flegyl,florazole,fossyol,giatricol,gineflavir,givagil,hydroxydimetridazole,hydroxymetronidazole,izoklion,klion,klont,mepagyl,meronidal,metric,metrolag,metrolyl,metromidol,metronidazolo,metronidazolum,metroplex,metrotop,mexibol,monagyl,monasin,nalox,nidagyl,noritate,novonidazol,nuvessa,orvagil,polibiotic,protostat,rathimed,rosaced,rosased,sanatrichom,satric,takimetol,trichazol,trichex,trichobrol,trichocide,trichomol,trichopal,trichopol,tricocet,tricom,trikacide,trikamon,trikhopol,trikojol,trikozol,trimeks,trivazol,vagilen,vagimid,vandazole,vertisal,wagitran,zadstat,zidoval</t>
         </is>
       </c>
       <c r="J271">
@@ -17444,7 +17444,7 @@
       </c>
       <c r="I277" t="inlineStr">
         <is>
-          <t>macropen,madecacine,medemycin,midecamicina,midecamycine,midecamycinum,midecin,momicine,mydecamycin,myoxam,normicina,rubimycin</t>
+          <t>macropen,madecacine,medemycin,midecamicina,midecamycine,midecamycinum,midecin,momicine,myoxam,normicina,rubimycin</t>
         </is>
       </c>
       <c r="J277">
@@ -17568,7 +17568,7 @@
       </c>
       <c r="I279" t="inlineStr">
         <is>
-          <t>acnez,arestin,borymycin,dynacin,lederderm,minociclina,minocin,minocline,minocyclin,minocyclinum,minocyn,minomax,minomycin,minoz,mynocine,periocline,solodyn,vectrin,ximino</t>
+          <t>acnez,arestin,borymycin,dynacin,lederderm,minociclina,minocin,minocline,minocyclin,minocyclinum,minocyn,minomax,minomycin,mynocine,periocline,solodyn,vectrin,ximino</t>
         </is>
       </c>
       <c r="J279">
@@ -18790,7 +18790,7 @@
       </c>
       <c r="I299" t="inlineStr">
         <is>
-          <t>alfuran,benkfuran,berkfuran,berkfurin,ceduran,chemiofuran,cistofuran,cyantin,cystit,dantafur,fuamed,furabid,furachel,furadantin,furadantine,furadantoin,furadoin,furadoine,furadonin,furadonine,furadoninum,furadontin,furalan,furaloid,furantoin,furantoina,furatoin,furedan,furina,furobactina,furodantin,gerofuran,ituran,macpac,macrobid,macrodantin,macrodantina,macrofuran,macrofurin,nierofu,nifuraden,nifuradene,nifuradeno,nifuradenum,nifuradine,nifurantin,nifuretten,nitoin,nitrex,nitrofuradantin,nitrofurantoina,nitrofurantoine,nitrofurantoinum,novofuran,orafuran,oxafuradene,oxafurandene,oxifuradene,oxyfuradene,parfuran,phenurin,renafur,siraliden,trantoin,uerineks,urantoin,urizept,urodin,urofuran,urofurin,urolisa,urolong,uvamin,welfurin,zoofurin</t>
+          <t>alfuran,benkfuran,berkfuran,berkfurin,ceduran,chemiofuran,cistofuran,cyantin,cystit,dantafur,fuamed,furabid,furachel,furadantin,furadantine,furadantoin,furadoin,furadoine,furadonin,furadonine,furadoninum,furadontin,furalan,furaloid,furantoina,furatoin,furedan,furina,furobactina,furodantin,gerofuran,ituran,macpac,macrobid,macrodantin,macrodantina,macrofuran,macrofurin,nierofu,nifuraden,nifuradene,nifuradeno,nifuradenum,nifuradine,nifurantin,nifuretten,nitoin,nitrex,nitrofuradantin,nitrofurantoina,nitrofurantoine,nitrofurantoinum,novofuran,orafuran,oxafuradene,oxafurandene,oxifuradene,oxyfuradene,parfuran,phenurin,renafur,siraliden,trantoin,uerineks,urizept,urodin,urofuran,urofurin,urolisa,urolong,uvamin,welfurin,zoofurin</t>
         </is>
       </c>
       <c r="J299">
@@ -18850,7 +18850,7 @@
       </c>
       <c r="I300" t="inlineStr">
         <is>
-          <t>acutol,aldomycin,alfucin,amifur,babrocid,becafurazone,biofuracina,biofurea,chemofuran,chixin,cocafurin,coxistat,dermofural,dymazone,dynazone,eldezol,fedacin,flavazone,fracine,furacilin,furacilinum,furacillin,furacin,furacine,furacinetten,furacoccid,furacort,furacycline,furaderm,furagent,furalcyn,furaldon,furalone,furametral,furaplast,furaseptyl,furaskin,furatsilin,furaziline,furazin,furazina,furazone,furazyme,furesol,furosem,fuvacillin,hemofuran,hydrazinecarboxamide,ibiofural,mammex,mastofuran,monafuracin,monafuracis,monofuracin,nefco,nifucin,nifurid,nifuzon,nitrofural,nitrofuralum,nitrofuran,nitrofurane,nitrofurazan,nitrofurazonum,nitrofurol,nitrozone,otofural,otofuran,rivafurazon,rivopon,sanfuran,semioxamazide,vabrocid,vadrocid,yatrocin</t>
+          <t>acutol,aldomycin,alfucin,amifur,babrocid,becafurazone,biofuracina,biofurea,chemofuran,chixin,cocafurin,coxistat,dermofural,dymazone,dynazone,eldezol,fedacin,flavazone,fracine,furacilin,furacilinum,furacillin,furacin,furacine,furacinetten,furacoccid,furacort,furacycline,furaderm,furagent,furalcyn,furaldon,furalone,furametral,furaplast,furaseptyl,furaskin,furatsilin,furaziline,furazin,furazina,furazyme,furesol,furosem,fuvacillin,hemofuran,hydrazinecarboxamide,ibiofural,mammex,mastofuran,monafuracin,monafuracis,monofuracin,nefco,nifucin,nifurid,nifuzon,nitrofural,nitrofuralum,nitrofuran,nitrofurane,nitrofurazan,nitrofurazonum,nitrofurol,nitrozone,otofural,otofuran,rivafurazon,rivopon,sanfuran,semioxamazide,vabrocid,vadrocid,yatrocin</t>
         </is>
       </c>
       <c r="J300" t="e">
@@ -18976,7 +18976,7 @@
       </c>
       <c r="I302" t="inlineStr">
         <is>
-          <t>baccidal,barazan,chibroxin,chibroxine,chibroxol,fulgram,gonorcin,lexinor,noflo,nolicin,noracin,noraxin,norflo,norfloxacine,norfloxacino,norfloxacinum,norocin,noroxin,noroxine,norxacin,sebercim,uroxacin,utinor,zoroxin</t>
+          <t>baccidal,barazan,chibroxin,chibroxine,chibroxol,fulgram,gonorcin,lexinor,nolicin,noracin,noraxin,norflo,norfloxacine,norfloxacino,norfloxacinum,norocin,noroxin,noroxine,norxacin,sebercim,uroxacin,utinor,zoroxin</t>
         </is>
       </c>
       <c r="J302">
@@ -19276,7 +19276,7 @@
       </c>
       <c r="I307" t="inlineStr">
         <is>
-          <t>albadry,albamix,albamycin,biotexin,cardelmycin,cardelmycinsalt,cathocin,cathomycin,inabiocin,inamycin,novobiocina,novobiocine,novobiocinsalt,novobiocinum,robiocina,sirbiocina,spheromycin,stilbiocina,streptonivicin,streptonivicinsalt,vulcamicina,vulcamycin,vulkamycin</t>
+          <t>albadry,albamix,albamycin,biotexin,cardelmycin,cardelmycinsalt,cathocin,cathomycin,inabiocin,novobiocina,novobiocine,novobiocinsalt,novobiocinum,robiocina,sirbiocina,spheromycin,stilbiocina,streptonivicin,streptonivicinsalt,vulcamicina,vulcamycin,vulkamycin</t>
         </is>
       </c>
       <c r="J307" t="e">
@@ -19334,7 +19334,7 @@
       </c>
       <c r="I308" t="inlineStr">
         <is>
-          <t>biofanal,diastatin,herniocid,moronal,myconystatin,mycostatin,mykostatyna,nilstat,nistatin,nistatina,nyotran,nystan,nystatyna,nystavescent,nystex,stamycin</t>
+          <t>biofanal,diastatin,herniocid,moronal,myconystatin,mycostatin,mykostatyna,nilstat,nistatin,nistatina,nyotran,nystan,nystatyna,nystavescent,nystex</t>
         </is>
       </c>
       <c r="J308">
@@ -19398,7 +19398,7 @@
       </c>
       <c r="I309" t="inlineStr">
         <is>
-          <t>exocin,exocine,flobacin,floxil,floxin,monoflocet,ocuflox,oflocet,ofloxacina,ofloxacine,ofloxacino,ofloxacinum,ofloxaxin,oxaldin,tarivid,visiren,zanocin</t>
+          <t>exocin,exocine,flobacin,floxil,floxin,monoflocet,oflocet,ofloxacina,ofloxacine,ofloxacino,ofloxacinum,ofloxaxin,oxaldin,tarivid,visiren,zanocin</t>
         </is>
       </c>
       <c r="J309">
@@ -19648,7 +19648,7 @@
       </c>
       <c r="I313" t="inlineStr">
         <is>
-          <t>aflukin,auriquin,biquinate,chinidin,chinidine,chinimetten,chinin,chinine,conchinin,conchinine,conquinine,dentojel,dihydrochinidin,dihydroquinidine,dihydroquinine,hydroconchinine,hydroconquinine,hydroquinidine,kinidin,numoquin,optochine,optoquine,pitayine,qualaquin,quinaglute,quine,quinicardine,quinidex,quinidine,quiniduran,quinindine,quinine,quinineanhydrous,quinora,quinsan,rezquin</t>
+          <t>aflukin,auriquin,biquinate,chinidin,chinidine,chinimetten,chinin,chinine,conchinin,conchinine,conquinine,dentojel,dihydrochinidin,dihydroquinidine,dihydroquinine,hydroconchinine,hydroconquinine,hydroquinidine,kinidin,numoquin,optochine,optoquine,pitayine,qualaquin,quinaglute,quinicardine,quinidex,quinidine,quiniduran,quinindine,quinine,quinineanhydrous,quinora,quinsan,rezquin</t>
         </is>
       </c>
       <c r="J313" t="e">
@@ -19888,7 +19888,7 @@
       </c>
       <c r="I317" t="inlineStr">
         <is>
-          <t>levornidazole,madelen,ornidal,ornidazol,ornidazolum,tiberal</t>
+          <t>levornidazole,madelen,ornidal,ornidazolum,tiberal</t>
         </is>
       </c>
       <c r="J317">
@@ -21296,7 +21296,7 @@
       </c>
       <c r="I340" t="inlineStr">
         <is>
-          <t>deblaston,dolcol,filtrax,karunomazin,memento,nuril,palin,pipedac,pipemid,pipemidate,pipemidic,pipemidicacid,pipram,pipurin,pyrido,tractur,uromidin,urosten,uroval</t>
+          <t>deblaston,dolcol,filtrax,karunomazin,memento,nuril,palin,pipedac,pipemid,pipemidate,pipemidic,pipemidicacid,pipram,pipurin,tractur,uromidin,urosten,uroval</t>
         </is>
       </c>
       <c r="J340">
@@ -21482,7 +21482,7 @@
       </c>
       <c r="I343" t="inlineStr">
         <is>
-          <t>piptazobactam,tazobac,tazonam,zobactin,zosyn</t>
+          <t>piptazobactam,tazonam,zobactin,zosyn</t>
         </is>
       </c>
       <c r="J343" t="e">
@@ -22156,7 +22156,7 @@
       </c>
       <c r="I354" t="inlineStr">
         <is>
-          <t>premafloxacine,premafloxacino,remafloxacin</t>
+          <t>premafloxacine,premafloxacino</t>
         </is>
       </c>
       <c r="J354" t="e">
@@ -22718,7 +22718,7 @@
       </c>
       <c r="I363" t="inlineStr">
         <is>
-          <t>aldinamid,aldinamide,eprazin,farmizina,isopas,novamid,pezetamid,piraldina,pirazimida,pirazinamid,pirazinamida,pirazinamide,pirazinecarboxamide,pyrafat,pyrazide,pyrazinamdie,pyrazinamid,pyrazinamidum,pyrazineamide,pyrizinamide,rifafour,rozide,tebrazid,tisamid,unipyranamide,zinamide</t>
+          <t>aldinamid,aldinamide,eprazin,farmizina,isopas,novamid,pezetamid,piraldina,pirazimida,pirazinamid,pirazinamida,pirazinamide,pirazinecarboxamide,pyrafat,pyrazide,pyrazinamdie,pyrazinamidum,pyrazineamide,pyrizinamide,rifafour,rozide,tebrazid,tisamid,unipyranamide</t>
         </is>
       </c>
       <c r="J363">
@@ -24566,7 +24566,7 @@
       </c>
       <c r="I393" t="inlineStr">
         <is>
-          <t>flagentyl,secnidal,secnidazol,secnidazolum,secnil,sindose,solosec</t>
+          <t>flagentyl,secnidal,secnidazolum,secnil,sindose,solosec</t>
         </is>
       </c>
       <c r="J393">
@@ -25686,7 +25686,7 @@
       </c>
       <c r="I411" t="inlineStr">
         <is>
-          <t>adiazin,adiazine,codiazine,cremodiazine,cremotres,debenal,deltazina,dermazin,dermazine,diazin,diazolone,diazovit,eskadiazine,flamazine,geben,liquadiazine,microsulfon,neazine,neotrizine,palatrize,piridisir,pirimal,pyrimal,quadetts,quadramoid,sanodiazine,silbertone,sildaflo,silvadene,silvazine,silver,silveramide,sliverex,solfadiazina,spofadrizine,sterazine,sulfacombin,sulfadiazene,sulfadiazin,sulfadiazina,sulfadiazinum,sulfapirimidin,sulfapyrimidin,sulfapyrimidine,sulfatryl,sulfazine,sulfolex,sulfonsol,sulfose,sulphadiazine,terfonyl,theradiazine,thermazene,trifonamide,trisem,truozine</t>
+          <t>codiazine,cremodiazine,cremotres,debenal,deltazina,dermazin,dermazine,diazolone,diazovit,eskadiazine,flamazine,geben,liquadiazine,microsulfon,neazine,neotrizine,palatrize,piridisir,pirimal,pyrimal,quadetts,quadramoid,sanodiazine,silbertone,sildaflo,silvadene,silvazine,silver,silveramide,sliverex,solfadiazina,spofadrizine,sterazine,sulfacombin,sulfadiazene,sulfadiazin,sulfadiazina,sulfadiazinum,sulfapirimidin,sulfapyrimidin,sulfapyrimidine,sulfatryl,sulfazine,sulfolex,sulfonsol,sulfose,sulphadiazine,terfonyl,theradiazine,thermazene,trifonamide,trisem,truozine</t>
         </is>
       </c>
       <c r="J411">
@@ -26064,7 +26064,7 @@
       </c>
       <c r="I417" t="inlineStr">
         <is>
-          <t>accuzole,alphazole,amidoxal,astrazolo,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,entusil,entusul,ganda,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazol,novazolo,novosaxazole,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxoxol,saxosozine,sodizole,solfafurazolo,sosol,soxamide,soxazole,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafurazol,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan</t>
+          <t>accuzole,alphazole,amidoxal,astrazolo,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,entusil,entusul,ganda,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazol,novazolo,novosaxazole,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxoxol,saxosozine,sodizole,solfafurazolo,sosol,soxamide,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafurazol,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan</t>
         </is>
       </c>
       <c r="J417">
@@ -26508,7 +26508,7 @@
       </c>
       <c r="I424" t="inlineStr">
         <is>
-          <t>aethazol,aethazolum,ayerlucil,berlophen,etazol,etazole,ethazole,famet,gliprotiazol,globucid,globucin,globuzid,glyprothiazol,glyprothiazole,glyprothiazolum,glyprothizolum,lucosil,methazol,microsul,proklar,renasul,rufol,salimol,sethadil,solfametizolo,solfetidolo,sulfaethidiole,sulfaethidol,sulfaethidole,sulfaethidolum,sulfaetidol,sulfamethizol,sulfamethizolum,sulfametizol,sulfapyelon,sulfstat,sulfurine,sulphaethidole,sulphamethizole,tardipyrine,tetracid,thidicur,thiosulfil,ultrasul,urocydal,urodiaton,urolucosil,urosulfin</t>
+          <t>aethazolum,ayerlucil,berlophen,gliprotiazol,globucid,globucin,globuzid,glyprothiazol,glyprothiazole,glyprothiazolum,glyprothizolum,lucosil,microsul,proklar,renasul,rufol,salimol,sethadil,solfametizolo,solfetidolo,sulfaethidiole,sulfaethidol,sulfaethidole,sulfaethidolum,sulfaetidol,sulfamethizol,sulfamethizolum,sulfametizol,sulfapyelon,sulfstat,sulfurine,sulphaethidole,sulphamethizole,tardipyrine,tetracid,thidicur,thiosulfil,ultrasul,urocydal,urodiaton,urolucosil,urosulfin</t>
         </is>
       </c>
       <c r="J424">
@@ -26572,7 +26572,7 @@
       </c>
       <c r="I425" t="inlineStr">
         <is>
-          <t>septran,septrin,simsinomin,sinomin,solfametossazolo,sulfamethalazole,sulfamethoxazol,sulfamethoxazolum,sulfamethoxizole,sulfamethylisoxazole,sulfametoxazol,sulfiodizole,sulfisomezole,sulphamethoxazol,sulphamethoxazole,sulphisomezole,urobak</t>
+          <t>septran,septrin,simsinomin,sinomin,solfametossazolo,sulfamethalazole,sulfamethoxazolum,sulfamethoxizole,sulfamethylisoxazole,sulfametoxazol,sulfiodizole,sulfisomezole,sulphisomezole,urobak</t>
         </is>
       </c>
       <c r="J425">
@@ -27872,7 +27872,7 @@
       </c>
       <c r="I446" t="inlineStr">
         <is>
-          <t>enmetazobactam,exblifep,tazobactamsalt,tazobactamum,tazobactum</t>
+          <t>exblifep,tazobactamsalt,tazobactamum,tazobactum</t>
         </is>
       </c>
       <c r="J446" t="e">
@@ -28620,7 +28620,7 @@
       </c>
       <c r="I458" t="inlineStr">
         <is>
-          <t>abramycin,abricycline,agromicina,ambramicina,ambramycin,amycin,biocycline,brodspec,cefracycline,centet,ciclibion,copharlan,criseociclina,cyclomycin,democracin,deschlorobiomycin,economycin,hostacyclin,lexacycline,limecycline,liquamycin,mericycline,micycline,neocycline,omegamycin,orlycycline,panmycin,purocyclina,roviciclina,solvocin,tetrabon,tetraciclina,tetracycl,tetracyclin,tetracyclinehydrate,tetracyclinum,tetracyn,tetradecin,tetrafil,tetraverine,tetrazyklin,tsiklomistsin,tsiklomitsin,veracin,vetacyclinum</t>
+          <t>abramycin,abricycline,agromicina,ambramicina,ambramycin,biocycline,brodspec,cefracycline,centet,ciclibion,copharlan,criseociclina,democracin,deschlorobiomycin,economycin,hostacyclin,lexacycline,limecycline,liquamycin,mericycline,micycline,neocycline,omegamycin,orlycycline,panmycin,purocyclina,roviciclina,solvocin,tetrabon,tetraciclina,tetracyclinehydrate,tetracyclinum,tetracyn,tetradecin,tetrafil,tetraverine,tetrazyklin,tsiklomistsin,tsiklomitsin,veracin,vetacyclinum</t>
         </is>
       </c>
       <c r="J458">
@@ -29170,7 +29170,7 @@
       </c>
       <c r="I467" t="inlineStr">
         <is>
-          <t>ticar,ticarcilina,ticarcilline,ticarcillinum,ticillin,timentin</t>
+          <t>ticar,ticarcilina,ticarcilline,ticarcillinum,timentin</t>
         </is>
       </c>
       <c r="J467" t="e">
@@ -29594,7 +29594,7 @@
       </c>
       <c r="I474" t="inlineStr">
         <is>
-          <t>amtiba,bioshik,fasigin,fasigyn,glongyn,haisigyn,isotinidazole,pletil,protozol,simplotan,sorquetan,symplotan,tindamax,tindazole,tinidazol,tinidazolum,tricolam,trimonase</t>
+          <t>amtiba,bioshik,fasigin,fasigyn,glongyn,haisigyn,isotinidazole,pletil,protozol,simplotan,sorquetan,symplotan,tindamax,tindazole,tinidazolum,tricolam,trimonase</t>
         </is>
       </c>
       <c r="J474">
@@ -29660,7 +29660,7 @@
       </c>
       <c r="I475" t="inlineStr">
         <is>
-          <t>aethoksid,aethoxyd,aethoxydum,amixyl,datanil,disocarban,disoxyl,ethoxide,ethoxyd,etocarlid,etocarlida,etocarlide,etocarlidum,etoksid,thiocarlide,tiocarlid,tiocarlida,tiocarlidum</t>
+          <t>aethoksid,aethoxydum,amixyl,datanil,disocarban,disoxyl,ethoxide,etocarlid,etocarlida,etocarlide,etocarlidum,etoksid,thiocarlide,tiocarlid,tiocarlida,tiocarlidum</t>
         </is>
       </c>
       <c r="J475">
@@ -29898,7 +29898,7 @@
       </c>
       <c r="I479" t="inlineStr">
         <is>
-          <t>aktob,bethkis,distobram,gotabiotic,kitabis,nebcin,nebicin,nebramycin,obramycin,tenebrimycin,tenemycin,tobacin,tobracin,tobradex,tobradistin,tobralex,tobramaxin,tobramicin,tobramicina,tobramitsetin,tobramycetin,tobramycine,tobramycinum,tobrased,tobrex</t>
+          <t>aktob,bethkis,distobram,gotabiotic,kitabis,nebcin,nebicin,nebramycin,tenebrimycin,tenemycin,tobacin,tobracin,tobradex,tobradistin,tobralex,tobramaxin,tobramicin,tobramicina,tobramitsetin,tobramycetin,tobramycine,tobramycinum,tobrased,tobrex</t>
         </is>
       </c>
       <c r="J479" t="e">
@@ -30080,7 +30080,7 @@
       </c>
       <c r="I482" t="inlineStr">
         <is>
-          <t>abaprim,anitrim,antrima,antrimox,bacdan,bacidal,bacide,bacin,bacta,bacterial,bacticel,bactifor,bactoprim,bactramin,bencole,bethaprim,biosulten,briscotrim,chemotrin,colizole,conprim,cotrimel,deprim,dosulfin,duocide,esbesul,espectrin,euctrim,exbesul,fermagex,fortrim,futin,ikaprim,infectotrimet,instalac,kombinax,lagatrim,lastrim,lescot,metoprim,monoprim,monotrim,monotrimin,novotrimel,omstat,pancidim,proloprim,protrin,purbal,resprim,roubac,roubal,salvatrim,setprin,sinotrim,stopan,streptoplus,sugaprim,sulfamar,sulfoxaprim,sulthrim,sultrex,syraprim,tiempe,toprim,trimethioprim,trimethoprime,trimethoprimum,trimethopriom,trimetoprim,trimetoprima,trimexol,trimezol,trimogal,trimono,trimopan,triprim,trisul,trisulcom,trisulfam,trisural,uretrim,urobactrim,utetrin,velaten,wellcoprim,wellcoprin,xeroprim,zamboprim</t>
+          <t>abaprim,anitrim,antrima,antrimox,bacdan,bacidal,bacide,bacin,bacterial,bacticel,bactifor,bactoprim,bactramin,bencole,bethaprim,biosulten,briscotrim,chemotrin,colizole,conprim,cotrimel,deprim,dosulfin,duocide,esbesul,espectrin,euctrim,exbesul,fermagex,fortrim,futin,ikaprim,infectotrimet,instalac,kombinax,lagatrim,lastrim,lescot,monoprim,monotrim,monotrimin,novotrimel,omstat,pancidim,proloprim,protrin,purbal,resprim,roubac,roubal,salvatrim,setprin,sinotrim,stopan,streptoplus,sugaprim,sulfamar,sulfoxaprim,sulthrim,sultrex,syraprim,tiempe,trimethioprim,trimethoprime,trimethoprimum,trimethopriom,trimetoprim,trimetoprima,trimexol,trimezol,trimogal,trimono,trimopan,triprim,trisul,trisulcom,trisulfam,trisural,uretrim,urobactrim,utetrin,velaten,wellcoprim,wellcoprin,xeroprim,zamboprim</t>
         </is>
       </c>
       <c r="J482">
@@ -30566,7 +30566,7 @@
       </c>
       <c r="I490" t="inlineStr">
         <is>
-          <t>ulifloxacin</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="J490" t="e">

</xml_diff>

<commit_message>
(v2.1.1.9270) Add support for Korean, fix ATCs
</commit_message>
<xml_diff>
--- a/data-raw/datasets/antimicrobials.xlsx
+++ b/data-raw/datasets/antimicrobials.xlsx
@@ -530,7 +530,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F3" t="e">
@@ -588,7 +588,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F4" t="e">
@@ -774,7 +774,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F7" t="e">
@@ -1045,17 +1045,21 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="J11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M11" t="e">
-        <v>#N/A</v>
+      <c r="J11">
+        <v>1.5</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1150,7 +1154,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F13" t="e">
@@ -1460,7 +1464,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F18" t="e">
@@ -1696,7 +1700,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F22" t="e">
@@ -1754,7 +1758,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F23" t="e">
@@ -1870,7 +1874,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F25" t="e">
@@ -2058,7 +2062,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA07,QJ01RA07</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2798,7 +2802,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F40" t="e">
@@ -2914,7 +2918,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F42" t="e">
@@ -3032,7 +3036,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F44" t="e">
@@ -3270,7 +3274,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F48" t="e">
@@ -4530,7 +4534,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F68" t="e">
@@ -4716,7 +4720,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F71" t="e">
@@ -5254,7 +5258,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F80" t="e">
@@ -5312,7 +5316,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F81" t="e">
@@ -5370,7 +5374,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F82" t="e">
@@ -6122,7 +6126,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F94" t="e">
@@ -6244,7 +6248,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F96" t="e">
@@ -6548,7 +6552,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F101" t="e">
@@ -6728,7 +6732,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F104" t="e">
@@ -6846,7 +6850,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F106" t="e">
@@ -7096,7 +7100,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F110" t="e">
@@ -7173,11 +7177,13 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="J111" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K111" t="e">
-        <v>#N/A</v>
+      <c r="J111">
+        <v>0.4</v>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="L111" t="e">
         <v>#N/A</v>
@@ -7462,7 +7468,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F116" t="e">
@@ -7520,7 +7526,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F117" t="e">
@@ -7545,13 +7551,11 @@
       <c r="K117" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L117">
-        <v>1.2</v>
-      </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+      <c r="L117" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M117" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N117" t="inlineStr">
         <is>
@@ -7580,7 +7584,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F118" t="e">
@@ -7727,11 +7731,13 @@
       <c r="K120" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L120" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M120" t="e">
-        <v>#N/A</v>
+      <c r="L120">
+        <v>6</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N120" t="inlineStr">
         <is>
@@ -7884,7 +7890,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F123" t="e">
@@ -8192,7 +8198,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F128" t="e">
@@ -8250,7 +8256,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F129" t="e">
@@ -8630,7 +8636,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F135" t="e">
@@ -8711,11 +8717,13 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="J136" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K136" t="e">
-        <v>#N/A</v>
+      <c r="J136">
+        <v>0.5</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="L136" t="e">
         <v>#N/A</v>
@@ -8750,7 +8758,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F137" t="e">
@@ -8808,7 +8816,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -8831,21 +8839,17 @@
           <t>anspor,cefradin,cefradina,cefradine,cefradinum,cekodin,cephradin,ecosporina,eskacef,infexin,megacef,sefril,velocef,velosef</t>
         </is>
       </c>
-      <c r="J138">
-        <v>2</v>
-      </c>
-      <c r="K138" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="L138">
-        <v>2</v>
-      </c>
-      <c r="M138" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+      <c r="J138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M138" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N138" t="inlineStr">
         <is>
@@ -8874,7 +8878,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F139" t="e">
@@ -9062,7 +9066,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F142" t="e">
@@ -9312,7 +9316,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA10,QJ01RA10</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -9374,7 +9378,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA12,QJ01RA12</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -9436,7 +9440,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA11,QJ01RA11</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -9564,7 +9568,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F150" t="e">
@@ -9622,7 +9626,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F151" t="e">
@@ -9746,7 +9750,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F153" t="e">
@@ -10248,7 +10252,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F161" t="e">
@@ -11254,7 +11258,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F177" t="e">
@@ -11494,7 +11498,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F181" t="e">
@@ -11618,7 +11622,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F183" t="e">
@@ -11936,7 +11940,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t/>
+          <t>J04AM03,QJ04AM03</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -12118,7 +12122,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F191" t="e">
@@ -12300,7 +12304,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F194" t="e">
@@ -12358,7 +12362,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F195" t="e">
@@ -12926,7 +12930,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F204" t="e">
@@ -13050,7 +13054,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F206" t="e">
@@ -13668,7 +13672,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F216" t="e">
@@ -13908,7 +13912,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F220" t="e">
@@ -14092,7 +14096,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F223" t="e">
@@ -14266,7 +14270,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t/>
+          <t>J01DH51,QJ01DH51</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -14330,7 +14334,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F227" t="e">
@@ -14388,7 +14392,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t/>
+          <t>J01DH56,QJ01DH56</t>
         </is>
       </c>
       <c r="F228" t="e">
@@ -14702,7 +14706,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -14960,7 +14964,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F237" t="e">
@@ -15018,7 +15022,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F238" t="e">
@@ -15442,7 +15446,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F245" t="e">
@@ -15566,7 +15570,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA05,QJ01RA05</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -15686,7 +15690,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F249" t="e">
@@ -15876,7 +15880,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F252" t="e">
@@ -16192,7 +16196,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F257" t="e">
@@ -16372,7 +16376,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F260" t="e">
@@ -16494,7 +16498,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F262" t="e">
@@ -16552,7 +16556,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t/>
+          <t>J01DH52,QJ01DH52</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -16616,7 +16620,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F264" t="e">
@@ -16932,7 +16936,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F269" t="e">
@@ -16990,7 +16994,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F270" t="e">
@@ -17178,7 +17182,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F273" t="e">
@@ -17490,7 +17494,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F278" t="e">
@@ -17678,7 +17682,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F281" t="e">
@@ -17922,7 +17926,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F285" t="e">
@@ -18098,7 +18102,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F288" t="e">
@@ -18220,7 +18224,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F290" t="e">
@@ -18530,7 +18534,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F295" t="e">
@@ -18588,7 +18592,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F296" t="e">
@@ -18834,7 +18838,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F300" t="e">
@@ -19020,7 +19024,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F303" t="e">
@@ -19078,7 +19082,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA14,QJ01RA14</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -19140,7 +19144,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA13,QJ01RA13</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -19202,7 +19206,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F306" t="e">
@@ -19444,7 +19448,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA09,QJ01RA09</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -19632,7 +19636,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F313" t="e">
@@ -19810,7 +19814,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F316" t="e">
@@ -20064,7 +20068,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F320" t="e">
@@ -20308,7 +20312,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F324" t="e">
@@ -20366,7 +20370,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F325" t="e">
@@ -20391,13 +20395,11 @@
       <c r="K325" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L325">
-        <v>2</v>
-      </c>
-      <c r="M325" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+      <c r="L325" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M325" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N325" t="inlineStr">
         <is>
@@ -20616,7 +20618,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F329" t="e">
@@ -20738,7 +20740,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F331" t="e">
@@ -20796,7 +20798,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F332" t="e">
@@ -20916,7 +20918,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F334" t="e">
@@ -20974,7 +20976,7 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F335" t="e">
@@ -21032,7 +21034,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F336" t="e">
@@ -21218,7 +21220,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F339" t="e">
@@ -21429,11 +21431,13 @@
       <c r="K342" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L342" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M342" t="e">
-        <v>#N/A</v>
+      <c r="L342">
+        <v>14</v>
+      </c>
+      <c r="M342" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N342" t="inlineStr">
         <is>
@@ -21526,7 +21530,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F344" t="e">
@@ -21958,7 +21962,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F351" t="e">
@@ -22140,7 +22144,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F354" t="e">
@@ -22262,7 +22266,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F356" t="e">
@@ -22512,7 +22516,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F360" t="e">
@@ -22762,7 +22766,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t/>
+          <t>QJ01FG02</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -22824,7 +22828,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F365" t="e">
@@ -22882,7 +22886,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F366" t="e">
@@ -22940,7 +22944,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F367" t="e">
@@ -23060,7 +23064,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F369" t="e">
@@ -23246,7 +23250,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F372" t="e">
@@ -23434,7 +23438,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t/>
+          <t>J04AM07,QJ04AM07</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
@@ -23496,7 +23500,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t/>
+          <t>J04AM02,QJ04AM02</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
@@ -23558,7 +23562,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t/>
+          <t>J04AM06,QJ04AM06</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -23620,7 +23624,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t/>
+          <t>J04AM05,QJ04AM05</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -23876,7 +23880,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F382" t="e">
@@ -23934,7 +23938,7 @@
       </c>
       <c r="E383" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F383" t="e">
@@ -24492,7 +24496,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F392" t="e">
@@ -24610,7 +24614,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t/>
+          <t>C10BA04,QC10BA04</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -25112,7 +25116,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA04,QJ01RA04</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -25302,7 +25306,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F405" t="e">
@@ -25360,7 +25364,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t/>
+          <t>J04AM01,QJ04AM01</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -25730,7 +25734,7 @@
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t/>
+          <t>J01EE06</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -25792,7 +25796,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t/>
+          <t>J01EE02,QJ01EW10,QJ51RE01</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -25982,7 +25986,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t/>
+          <t>J01EE05,QJ01EW03</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -26368,7 +26372,7 @@
       </c>
       <c r="E422" t="inlineStr">
         <is>
-          <t/>
+          <t>J01EE07,QJ01EW18</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
@@ -26430,7 +26434,7 @@
       </c>
       <c r="E423" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F423" t="e">
@@ -26806,7 +26810,7 @@
       </c>
       <c r="E429" t="inlineStr">
         <is>
-          <t/>
+          <t>J01EE03</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
@@ -26934,7 +26938,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t/>
+          <t>J01EE04</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
@@ -27250,7 +27254,7 @@
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F436" t="e">
@@ -27434,7 +27438,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F439" t="e">
@@ -27492,7 +27496,7 @@
       </c>
       <c r="E440" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F440" t="e">
@@ -27550,7 +27554,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F441" t="e">
@@ -27672,7 +27676,7 @@
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F443" t="e">
@@ -27794,7 +27798,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F445" t="e">
@@ -27914,7 +27918,7 @@
       </c>
       <c r="E447" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F447" t="e">
@@ -27933,13 +27937,11 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="J447">
-        <v>0.56</v>
-      </c>
-      <c r="K447" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+      <c r="J447" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K447" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L447" t="e">
         <v>#N/A</v>
@@ -28104,7 +28106,7 @@
       </c>
       <c r="E450" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F450" t="e">
@@ -28666,7 +28668,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F459" t="e">
@@ -28724,7 +28726,7 @@
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t/>
+          <t>J01RA08,QJ01RA08</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
@@ -28786,7 +28788,7 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F461" t="e">
@@ -28844,7 +28846,7 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F462" t="e">
@@ -29030,7 +29032,7 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t/>
+          <t>J04AM04,QJ04AM04</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
@@ -29342,7 +29344,7 @@
       </c>
       <c r="E470" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F470" t="e">
@@ -29704,7 +29706,7 @@
       </c>
       <c r="E476" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F476" t="e">
@@ -29762,7 +29764,7 @@
       </c>
       <c r="E477" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F477" t="e">
@@ -29820,7 +29822,7 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F478" t="e">
@@ -29942,7 +29944,7 @@
       </c>
       <c r="E480" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F480" t="e">
@@ -30126,7 +30128,7 @@
       </c>
       <c r="E483" t="inlineStr">
         <is>
-          <t/>
+          <t>J01EE01</t>
         </is>
       </c>
       <c r="F483" t="inlineStr">
@@ -30252,7 +30254,7 @@
       </c>
       <c r="E485" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F485" t="e">
@@ -30550,7 +30552,7 @@
       </c>
       <c r="E490" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F490" t="e">
@@ -30674,7 +30676,7 @@
       </c>
       <c r="E492" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F492" t="e">
@@ -30732,7 +30734,7 @@
       </c>
       <c r="E493" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F493" t="e">
@@ -30790,7 +30792,7 @@
       </c>
       <c r="E494" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F494" t="e">
@@ -30976,7 +30978,7 @@
       </c>
       <c r="E497" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F497" t="e">
@@ -31032,7 +31034,7 @@
       </c>
       <c r="E498" t="inlineStr">
         <is>
-          <t/>
+          <t>NA</t>
         </is>
       </c>
       <c r="F498" t="e">

</xml_diff>

<commit_message>
(v2.1.1.9272) (v2.1.1.9271) add sensititre AB and animal codes
</commit_message>
<xml_diff>
--- a/data-raw/datasets/antimicrobials.xlsx
+++ b/data-raw/datasets/antimicrobials.xlsx
@@ -725,7 +725,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>ak,ami,amik,amk,an</t>
+          <t>ak,ami,amik,amikac,amk,an</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -909,7 +909,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ac,amox,amx</t>
+          <t>ac,amox,amoxic,amx</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -975,7 +975,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>a/c,amcl,aml,aug,xl</t>
+          <t>a/c,amcl,aml,amocla,aug,xl</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>amf,amfb,amph</t>
+          <t>amf,amfb,amph,amphot</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>am,amp,ampi</t>
+          <t>am,amp,amp100,amp200,ampi,ampici</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>a/s,ab,ams,amsu,apsu,sam</t>
+          <t>a/s,ab,ampsul,ams,amsu,apsu,sam</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>anid</t>
+          <t>anid,anidul</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>apalci</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>apramy</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>arbeka</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>apoxic,aspoxi</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>astrom</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>avilam</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>az,azi,azit,azm</t>
+          <t>az,azi,azit,azithr,azm</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2139,7 +2139,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>az,azl,azlo</t>
+          <t>az,azl,azlo,azloci</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>at,atm,azm,azt,aztr</t>
+          <t>at,atm,azm,azt,azt1,aztr,aztreo</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>bacamp</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2443,7 +2443,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>baci</t>
+          <t>baci,bacitr</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>bepe,pen,peni,peni g,penicillin,penicillin g,pg</t>
+          <t>bepe,pen,peni,peni g,penic8,penica,penici,penicillin,penicillin g,penora,pg</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2871,7 +2871,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>besifl</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>biapen</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>capr</t>
+          <t>capr,capreo</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3475,7 +3475,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>bar,carb,cb</t>
+          <t>bar,carb,carben,cb</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>casp</t>
+          <t>casp,caspof</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -3727,7 +3727,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cephac</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>ccl,cec,cf,cfac,cfc,cfcl,cfr,fac</t>
+          <t>ccl,cec,cefacl,cf,cfac,cfc,cfcl,cfr,fac</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -3853,7 +3853,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>cfdx,cfr,fad</t>
+          <t>cefadr,cfdx,cfr,fad</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>cflx</t>
+          <t>cepale,cflx</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -3981,7 +3981,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>cefa</t>
+          <t>cefa,ceplor</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>cfal,cflt</t>
+          <t>cephal,cfal,cflt</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>cfam,cfmn</t>
+          <t>cefama,cfam,cfmn</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cephap</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -4237,7 +4237,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefatr</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -4301,7 +4301,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefaze</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -4365,7 +4365,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>cfz,cfzl,cz,czol,faz,kz</t>
+          <t>cefazo,cfz,cfzl,cz,czol,faz,kz</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefbup</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -4485,7 +4485,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefcap</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -4607,7 +4607,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>cd,cdn,cdr,cfd,din</t>
+          <t>cd,cdn,cdr,cefdin,cfd,din</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -4671,7 +4671,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>cdn</t>
+          <t>cdn,cefdit</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>cfep,cfpi,cpe,cpm,fep,pm,xpm</t>
+          <t>cefep4,cefepi,cfep,cfpi,cpe,cpm,fep,pm,xpm</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -4915,7 +4915,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>cicl,xpml</t>
+          <t>cefcla,cicl,xpml</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -5209,7 +5209,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefeta,cefmtm</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -5507,7 +5507,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>cfe,cfix,cfxm,dcfm,fix,ix</t>
+          <t>cefixi,cfe,cfix,cfxm,dcfm,fix,ix</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefmen</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -5697,7 +5697,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefmet</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -5757,7 +5757,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefmin</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefoni</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -5949,7 +5949,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>cfp,cfpz,cp,cpz,fop,per</t>
+          <t>cefope,cfp,cfpz,cp,cpz,fop,per</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>fopsul</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefora</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefose</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -6199,7 +6199,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>cfot,cft,cftx,ct,ctx,fot,tax,xct</t>
+          <t>cefo32,cefota,cfot,cft,cftx,ct,ctx,fot,fot1,tax,taxmen,taxnme,xct</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>cxcl,xctl</t>
+          <t>cxcl,taxcla,xctl</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -6437,7 +6437,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>cftt,cn,cte,ctn,ctt,tans</t>
+          <t>cefote,cftt,cn,cte,ctn,ctt,tans</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -6501,7 +6501,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefoti</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -6621,7 +6621,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefove</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -6683,7 +6683,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>cfox,cfx,cfxt,cx,fox,fx</t>
+          <t>cefoxi,cfox,cfx,cfxt,cx,fox,fx</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -6801,7 +6801,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefozo</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
@@ -6861,7 +6861,7 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefpim</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
@@ -6923,7 +6923,7 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefpam</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
@@ -6987,7 +6987,7 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>cfpr</t>
+          <t>cefpom,cfpr</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
@@ -7051,7 +7051,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>cfpd,cfpo,cpd,pod,px</t>
+          <t>cefpod,cfpd,cfpo,cpd,pod,pod4,px</t>
         </is>
       </c>
       <c r="I109" t="inlineStr">
@@ -7169,7 +7169,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>cecl</t>
+          <t>cecl,podcla</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
@@ -7233,7 +7233,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>cpr,cpz,fp</t>
+          <t>cefpro,cpr,cpz,fp</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -7293,7 +7293,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefqui</t>
         </is>
       </c>
       <c r="I113" t="inlineStr">
@@ -7355,7 +7355,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>ceftix</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
@@ -7419,7 +7419,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>cfsl,cfsu</t>
+          <t>cefsul,cfsl,cfsu</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
@@ -7537,7 +7537,7 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>cfro</t>
+          <t>ceftar,cfro</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
@@ -7657,7 +7657,7 @@
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>caz,cefta,cfta,cftz,taz,tz,xtz</t>
+          <t>caz,cefta,ceftaz,cfta,cftz,taz,tz,xtz</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
@@ -7781,7 +7781,7 @@
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>czcl,xtzl</t>
+          <t>czcl,tazcla,xtzl</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
@@ -7841,7 +7841,7 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefter</t>
         </is>
       </c>
       <c r="I122" t="inlineStr">
@@ -7963,7 +7963,7 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>ceftez</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
@@ -8027,7 +8027,7 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>cb,cfbu,ctb,tib</t>
+          <t>cb,ceftib,cfbu,ctb,tib</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
@@ -8087,7 +8087,7 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>ceftif</t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
@@ -8149,7 +8149,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>cfzx,ctz,cz,czx,tiz,zox</t>
+          <t>ceftiz,cfzx,ctz,cz,czx,tiz,zox</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
@@ -8267,7 +8267,7 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>ceftob</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -8457,7 +8457,7 @@
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>axo,cax,cftr,cro,ctr,frx,tx</t>
+          <t>axo,cax,ceftri,cftr,cro,ctr,frx,trimen,trinme,tx</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
@@ -8585,7 +8585,7 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>cfrx,cfur,cfx,crm,cxm,fur,rox,xm</t>
+          <t>cefaxe,cefrox,cefuro,cfrx,cfur,cfx,crm,cxm,fur,rox,xm</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
@@ -8769,7 +8769,7 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cefuzo</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
@@ -8831,7 +8831,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>cfra,cfrd</t>
+          <t>cephra,cfra,cfrd</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -8951,7 +8951,7 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>c,chl,chlo,cl</t>
+          <t>c,chl,chlo,chlora,cl</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
@@ -9017,7 +9017,7 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>chltet</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
@@ -9077,7 +9077,7 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>cyclac</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -9201,7 +9201,7 @@
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>cino,cnox</t>
+          <t>cino,cinoxa,cnox</t>
         </is>
       </c>
       <c r="I144" t="inlineStr">
@@ -9265,7 +9265,7 @@
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>ci,cip,cipr,cp</t>
+          <t>ci,cip,cipr,ciprof,cp</t>
         </is>
       </c>
       <c r="I145" t="inlineStr">
@@ -9517,7 +9517,7 @@
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>ch,cla,clar,clm,clr</t>
+          <t>ch,cla,clar,claryt,clm,clr</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
@@ -9637,7 +9637,7 @@
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>clinaf</t>
         </is>
       </c>
       <c r="I151" t="inlineStr">
@@ -9699,7 +9699,7 @@
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>cc,cd,cli,clin,cm,da</t>
+          <t>cc,cd,cli,clin,clin32,clinda,cm,da</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
@@ -9823,7 +9823,7 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>clof</t>
+          <t>clof,clofam</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
@@ -10135,7 +10135,7 @@
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>clox</t>
+          <t>clox,cloxac</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
@@ -10201,7 +10201,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>cl,coli,cs,cst,ct</t>
+          <t>cl,coli,colist,cs,cst,ct</t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
@@ -10325,7 +10325,7 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>cycl</t>
+          <t>cycl,cyclos</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
@@ -10389,7 +10389,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>dalb</t>
+          <t>dalb,dalbav</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
@@ -10449,7 +10449,7 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>danofl</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
@@ -10575,7 +10575,7 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>dap,dapt</t>
+          <t>dap,dapt,dapt25,dapt50,daptom</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
@@ -10765,7 +10765,7 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>demecy</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
@@ -10829,7 +10829,7 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>dibeka</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
@@ -10893,7 +10893,7 @@
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>dicl</t>
+          <t>dicl,diclox</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
@@ -10955,7 +10955,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>diflox</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
@@ -11017,7 +11017,7 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>dirith</t>
         </is>
       </c>
       <c r="I173" t="inlineStr">
@@ -11081,7 +11081,7 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>dori</t>
+          <t>dori,doripe</t>
         </is>
       </c>
       <c r="I174" t="inlineStr">
@@ -11145,7 +11145,7 @@
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>dox,doxy</t>
+          <t>dox,doxy,doxycy</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
@@ -11331,7 +11331,7 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>enox</t>
+          <t>enox,enoxa</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
@@ -11391,7 +11391,7 @@
       </c>
       <c r="H179" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>enrofl</t>
         </is>
       </c>
       <c r="I179" t="inlineStr">
@@ -11759,7 +11759,7 @@
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>erta,etp</t>
+          <t>erta,ertape,etp</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
@@ -11823,7 +11823,7 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>e,em,ery,eryt</t>
+          <t>e,em,ery,ery32,eryt,eryth</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
@@ -11889,7 +11889,7 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>etha</t>
+          <t>etha,ethamb</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
@@ -12017,7 +12017,7 @@
       </c>
       <c r="H189" t="inlineStr">
         <is>
-          <t>ethi</t>
+          <t>ethi,ethion</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
@@ -12195,7 +12195,7 @@
       </c>
       <c r="H192" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>farope</t>
         </is>
       </c>
       <c r="I192" t="inlineStr">
@@ -12373,7 +12373,7 @@
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>flavom</t>
         </is>
       </c>
       <c r="I195" t="inlineStr">
@@ -12435,7 +12435,7 @@
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>fler</t>
+          <t>fler,flerox</t>
         </is>
       </c>
       <c r="I196" t="inlineStr">
@@ -12497,7 +12497,7 @@
       </c>
       <c r="H197" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>flomox</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
@@ -12557,7 +12557,7 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>florfe</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
@@ -12619,7 +12619,7 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>clox,flux</t>
+          <t>clox,fluclo,flux</t>
         </is>
       </c>
       <c r="I199" t="inlineStr">
@@ -12685,7 +12685,7 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>fluc,fluz,flz</t>
+          <t>fluc,flucon,fluz,flz</t>
         </is>
       </c>
       <c r="I200" t="inlineStr">
@@ -12751,7 +12751,7 @@
       </c>
       <c r="H201" t="inlineStr">
         <is>
-          <t>5flc,fcu,fluo,fluy</t>
+          <t>5flc,fcu,flucyt,fluo,fluy</t>
         </is>
       </c>
       <c r="I201" t="inlineStr">
@@ -12817,7 +12817,7 @@
       </c>
       <c r="H202" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>flumeq</t>
         </is>
       </c>
       <c r="I202" t="inlineStr">
@@ -13003,7 +13003,7 @@
       </c>
       <c r="H205" t="inlineStr">
         <is>
-          <t>ff,fm,fo,fof,fos,fosf</t>
+          <t>ff,fm,fo,fof,fos,fosf,fosfom,fosmyc</t>
         </is>
       </c>
       <c r="I205" t="inlineStr">
@@ -13123,7 +13123,7 @@
       </c>
       <c r="H207" t="inlineStr">
         <is>
-          <t>fram</t>
+          <t>fram,framyc</t>
         </is>
       </c>
       <c r="I207" t="inlineStr">
@@ -13245,7 +13245,7 @@
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>furazo</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">
@@ -13307,7 +13307,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>fa,fusi</t>
+          <t>fa,fusaci,fusi</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
@@ -13427,7 +13427,7 @@
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>gareno</t>
         </is>
       </c>
       <c r="I212" t="inlineStr">
@@ -13491,7 +13491,7 @@
       </c>
       <c r="H213" t="inlineStr">
         <is>
-          <t>gati</t>
+          <t>gati,gatifl</t>
         </is>
       </c>
       <c r="I213" t="inlineStr">
@@ -13557,7 +13557,7 @@
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>gemifl</t>
         </is>
       </c>
       <c r="I214" t="inlineStr">
@@ -13623,7 +13623,7 @@
       </c>
       <c r="H215" t="inlineStr">
         <is>
-          <t>cn,gen,gent,gm</t>
+          <t>cn,ge1000,ge2000,gen,gen128,gen500,gent,genta1,gentam,gm</t>
         </is>
       </c>
       <c r="I215" t="inlineStr">
@@ -13803,7 +13803,7 @@
       </c>
       <c r="H218" t="inlineStr">
         <is>
-          <t>grep</t>
+          <t>grep,grepaf</t>
         </is>
       </c>
       <c r="I218" t="inlineStr">
@@ -14047,7 +14047,7 @@
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>hetaci</t>
         </is>
       </c>
       <c r="I222" t="inlineStr">
@@ -14223,7 +14223,7 @@
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>iclapr</t>
         </is>
       </c>
       <c r="I225" t="inlineStr">
@@ -14285,7 +14285,7 @@
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>imci,imi,imip,imp</t>
+          <t>imci,imi,imip,imip32,imipen,imp</t>
         </is>
       </c>
       <c r="I226" t="inlineStr">
@@ -14529,7 +14529,7 @@
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>isepam</t>
         </is>
       </c>
       <c r="I230" t="inlineStr">
@@ -14655,7 +14655,7 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>inh</t>
+          <t>inh,isonia</t>
         </is>
       </c>
       <c r="I232" t="inlineStr">
@@ -14783,7 +14783,7 @@
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>itra</t>
+          <t>itra,itraco</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
@@ -14849,7 +14849,7 @@
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>josamy</t>
         </is>
       </c>
       <c r="I235" t="inlineStr">
@@ -14913,7 +14913,7 @@
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>hlk,k,kan,kana,km</t>
+          <t>hlk,k,kan,kana,kanamy,km</t>
         </is>
       </c>
       <c r="I236" t="inlineStr">
@@ -15095,7 +15095,7 @@
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>keto,ktc</t>
+          <t>keto,ketoco,ktc</t>
         </is>
       </c>
       <c r="I239" t="inlineStr">
@@ -15519,7 +15519,7 @@
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>le,lev,levo,lvx</t>
+          <t>le,lev,levo,levofl,lvx</t>
         </is>
       </c>
       <c r="I246" t="inlineStr">
@@ -15763,7 +15763,7 @@
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>linc</t>
+          <t>linc,lincom</t>
         </is>
       </c>
       <c r="I250" t="inlineStr">
@@ -15829,7 +15829,7 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>line,lnz,lz,lzd</t>
+          <t>line,linezo,lnz,lz,lzd</t>
         </is>
       </c>
       <c r="I251" t="inlineStr">
@@ -15891,7 +15891,7 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>linflo</t>
         </is>
       </c>
       <c r="I252" t="inlineStr">
@@ -15953,7 +15953,7 @@
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>lmf,lom,lome</t>
+          <t>lmf,lom,lome,lomefl</t>
         </is>
       </c>
       <c r="I253" t="inlineStr">
@@ -16017,7 +16017,7 @@
       </c>
       <c r="H254" t="inlineStr">
         <is>
-          <t>lora</t>
+          <t>lora,loraca</t>
         </is>
       </c>
       <c r="I254" t="inlineStr">
@@ -16265,7 +16265,7 @@
       </c>
       <c r="H258" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>marbof</t>
         </is>
       </c>
       <c r="I258" t="inlineStr">
@@ -16327,7 +16327,7 @@
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>amdinocillin</t>
+          <t>amdinocillin,mecill</t>
         </is>
       </c>
       <c r="I259" t="inlineStr">
@@ -16449,7 +16449,7 @@
       </c>
       <c r="H261" t="inlineStr">
         <is>
-          <t>mem,mer,mero,mp,mrp</t>
+          <t>mem,mer,mero,merope,mp,mrp</t>
         </is>
       </c>
       <c r="I261" t="inlineStr">
@@ -16693,7 +16693,7 @@
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>methcy</t>
         </is>
       </c>
       <c r="I265" t="inlineStr">
@@ -16887,7 +16887,7 @@
       </c>
       <c r="H268" t="inlineStr">
         <is>
-          <t>meti</t>
+          <t>methic,meti</t>
         </is>
       </c>
       <c r="I268" t="inlineStr">
@@ -17067,7 +17067,7 @@
       </c>
       <c r="H271" t="inlineStr">
         <is>
-          <t>metr,mnz</t>
+          <t>metr,metron,mnz</t>
         </is>
       </c>
       <c r="I271" t="inlineStr">
@@ -17133,7 +17133,7 @@
       </c>
       <c r="H272" t="inlineStr">
         <is>
-          <t>mez,mezl,mz</t>
+          <t>mez,mezl,mezlo,mz</t>
         </is>
       </c>
       <c r="I272" t="inlineStr">
@@ -17193,7 +17193,7 @@
       </c>
       <c r="H273" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>mezsul</t>
         </is>
       </c>
       <c r="I273" t="inlineStr">
@@ -17255,7 +17255,7 @@
       </c>
       <c r="H274" t="inlineStr">
         <is>
-          <t>mica</t>
+          <t>mica,micafu</t>
         </is>
       </c>
       <c r="I274" t="inlineStr">
@@ -17381,7 +17381,7 @@
       </c>
       <c r="H276" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>micron</t>
         </is>
       </c>
       <c r="I276" t="inlineStr">
@@ -17443,7 +17443,7 @@
       </c>
       <c r="H277" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>mideka</t>
         </is>
       </c>
       <c r="I277" t="inlineStr">
@@ -17505,7 +17505,7 @@
       </c>
       <c r="H278" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>amiflo</t>
         </is>
       </c>
       <c r="I278" t="inlineStr">
@@ -17567,7 +17567,7 @@
       </c>
       <c r="H279" t="inlineStr">
         <is>
-          <t>mc,mh,mi,min,mino,mn,mno</t>
+          <t>mc,mh,mi,min,mino,minocy,mn,mno</t>
         </is>
       </c>
       <c r="I279" t="inlineStr">
@@ -17817,7 +17817,7 @@
       </c>
       <c r="H283" t="inlineStr">
         <is>
-          <t>mox,moxi,mxf</t>
+          <t>mox,moxi,moxifl,mxf</t>
         </is>
       </c>
       <c r="I283" t="inlineStr">
@@ -17879,7 +17879,7 @@
       </c>
       <c r="H284" t="inlineStr">
         <is>
-          <t>mup,mupi</t>
+          <t>mup,mupi,mupiro</t>
         </is>
       </c>
       <c r="I284" t="inlineStr">
@@ -18053,7 +18053,7 @@
       </c>
       <c r="H287" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>nafcil</t>
         </is>
       </c>
       <c r="I287" t="inlineStr">
@@ -18175,7 +18175,7 @@
       </c>
       <c r="H289" t="inlineStr">
         <is>
-          <t>na,nal,nali</t>
+          <t>na,nal,nalac,nali</t>
         </is>
       </c>
       <c r="I289" t="inlineStr">
@@ -18293,7 +18293,7 @@
       </c>
       <c r="H291" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>narasi</t>
         </is>
       </c>
       <c r="I291" t="inlineStr">
@@ -18417,7 +18417,7 @@
       </c>
       <c r="H293" t="inlineStr">
         <is>
-          <t>neom</t>
+          <t>neom,neomyc</t>
         </is>
       </c>
       <c r="I293" t="inlineStr">
@@ -18483,7 +18483,7 @@
       </c>
       <c r="H294" t="inlineStr">
         <is>
-          <t>neti</t>
+          <t>neti,netilm</t>
         </is>
       </c>
       <c r="I294" t="inlineStr">
@@ -18789,7 +18789,7 @@
       </c>
       <c r="H299" t="inlineStr">
         <is>
-          <t>f,f/m,fd,ft,ni,nit,nitr</t>
+          <t>f,f/m,fd,ft,ni,nit,nit16,nitr,nitro</t>
         </is>
       </c>
       <c r="I299" t="inlineStr">
@@ -18849,7 +18849,7 @@
       </c>
       <c r="H300" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>nitfur</t>
         </is>
       </c>
       <c r="I300" t="inlineStr">
@@ -18975,7 +18975,7 @@
       </c>
       <c r="H302" t="inlineStr">
         <is>
-          <t>nor,norf,nx,nxn</t>
+          <t>nor,norf,norflo,nx,nxn</t>
         </is>
       </c>
       <c r="I302" t="inlineStr">
@@ -19275,7 +19275,7 @@
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>novo</t>
+          <t>novo,novobi</t>
         </is>
       </c>
       <c r="I307" t="inlineStr">
@@ -19333,7 +19333,7 @@
       </c>
       <c r="H308" t="inlineStr">
         <is>
-          <t>nyst</t>
+          <t>nyst,nystan</t>
         </is>
       </c>
       <c r="I308" t="inlineStr">
@@ -19397,7 +19397,7 @@
       </c>
       <c r="H309" t="inlineStr">
         <is>
-          <t>of,ofl,oflo,ofx</t>
+          <t>of,ofl,oflo,ofloxa,ofx</t>
         </is>
       </c>
       <c r="I309" t="inlineStr">
@@ -19525,7 +19525,7 @@
       </c>
       <c r="H311" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>oleand</t>
         </is>
       </c>
       <c r="I311" t="inlineStr">
@@ -19705,7 +19705,7 @@
       </c>
       <c r="H314" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>orbifl</t>
         </is>
       </c>
       <c r="I314" t="inlineStr">
@@ -19767,7 +19767,7 @@
       </c>
       <c r="H315" t="inlineStr">
         <is>
-          <t>orit</t>
+          <t>orit,oritav</t>
         </is>
       </c>
       <c r="I315" t="inlineStr">
@@ -20017,7 +20017,7 @@
       </c>
       <c r="H319" t="inlineStr">
         <is>
-          <t>ox,oxa,oxac,oxal,oxs</t>
+          <t>ox,oxa,oxac,oxacil,oxal,oxs</t>
         </is>
       </c>
       <c r="I319" t="inlineStr">
@@ -20141,7 +20141,7 @@
       </c>
       <c r="H321" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>oxoaci</t>
         </is>
       </c>
       <c r="I321" t="inlineStr">
@@ -20205,7 +20205,7 @@
       </c>
       <c r="H322" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>oxytet</t>
         </is>
       </c>
       <c r="I322" t="inlineStr">
@@ -20323,7 +20323,7 @@
       </c>
       <c r="H324" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>pasraa</t>
         </is>
       </c>
       <c r="I324" t="inlineStr">
@@ -20567,7 +20567,7 @@
       </c>
       <c r="H328" t="inlineStr">
         <is>
-          <t>pefl</t>
+          <t>pefl,perflo</t>
         </is>
       </c>
       <c r="I328" t="inlineStr">
@@ -20751,7 +20751,7 @@
       </c>
       <c r="H331" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>pennov</t>
         </is>
       </c>
       <c r="I331" t="inlineStr">
@@ -21171,7 +21171,7 @@
       </c>
       <c r="H338" t="inlineStr">
         <is>
-          <t>fepe,peni v,penicillin v,pnv,pv</t>
+          <t>fepe,peni v,penicillin v,phepen,pnv,pv</t>
         </is>
       </c>
       <c r="I338" t="inlineStr">
@@ -21293,7 +21293,7 @@
       </c>
       <c r="H340" t="inlineStr">
         <is>
-          <t>pipz,pizu</t>
+          <t>pipaci,pipz,pizu</t>
         </is>
       </c>
       <c r="I340" t="inlineStr">
@@ -21357,7 +21357,7 @@
       </c>
       <c r="H341" t="inlineStr">
         <is>
-          <t>pi,pip,pipc,pipe,pp</t>
+          <t>pi,pip,pipc,pipe,pipera,pp</t>
         </is>
       </c>
       <c r="I341" t="inlineStr">
@@ -21599,7 +21599,7 @@
       </c>
       <c r="H345" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>pirlim</t>
         </is>
       </c>
       <c r="I345" t="inlineStr">
@@ -21789,7 +21789,7 @@
       </c>
       <c r="H348" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>pivmec</t>
         </is>
       </c>
       <c r="I348" t="inlineStr">
@@ -21911,7 +21911,7 @@
       </c>
       <c r="H350" t="inlineStr">
         <is>
-          <t>pb,pol,polb,poly,poly b,polymixin,polymixin b</t>
+          <t>pb,pol,polb,poly,poly b,polyb,polymixin,polymixin b</t>
         </is>
       </c>
       <c r="I350" t="inlineStr">
@@ -22035,7 +22035,7 @@
       </c>
       <c r="H352" t="inlineStr">
         <is>
-          <t>posa</t>
+          <t>posa,posaco</t>
         </is>
       </c>
       <c r="I352" t="inlineStr">
@@ -22155,7 +22155,7 @@
       </c>
       <c r="H354" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>premaf</t>
         </is>
       </c>
       <c r="I354" t="inlineStr">
@@ -22339,7 +22339,7 @@
       </c>
       <c r="H357" t="inlineStr">
         <is>
-          <t>pris</t>
+          <t>pris,pristi</t>
         </is>
       </c>
       <c r="I357" t="inlineStr">
@@ -22781,7 +22781,7 @@
       </c>
       <c r="H364" t="inlineStr">
         <is>
-          <t>q/d,qda,qida,quda,rp,syn</t>
+          <t>q/d,qda,qida,quda,rp,syn,synerc</t>
         </is>
       </c>
       <c r="I364" t="inlineStr">
@@ -22897,7 +22897,7 @@
       </c>
       <c r="H366" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>ramopl</t>
         </is>
       </c>
       <c r="I366" t="inlineStr">
@@ -22955,7 +22955,7 @@
       </c>
       <c r="H367" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>razupe</t>
         </is>
       </c>
       <c r="I367" t="inlineStr">
@@ -23323,7 +23323,7 @@
       </c>
       <c r="H373" t="inlineStr">
         <is>
-          <t>rifb</t>
+          <t>ansamy,rifb</t>
         </is>
       </c>
       <c r="I373" t="inlineStr">
@@ -23387,7 +23387,7 @@
       </c>
       <c r="H374" t="inlineStr">
         <is>
-          <t>rifa</t>
+          <t>rifa,rifamp</t>
         </is>
       </c>
       <c r="I374" t="inlineStr">
@@ -23701,7 +23701,7 @@
       </c>
       <c r="H379" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>rifmyc</t>
         </is>
       </c>
       <c r="I379" t="inlineStr">
@@ -24011,7 +24011,7 @@
       </c>
       <c r="H384" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>rokita</t>
         </is>
       </c>
       <c r="I384" t="inlineStr">
@@ -24203,7 +24203,7 @@
       </c>
       <c r="H387" t="inlineStr">
         <is>
-          <t>roxi</t>
+          <t>roxi,roxith</t>
         </is>
       </c>
       <c r="I387" t="inlineStr">
@@ -24327,7 +24327,7 @@
       </c>
       <c r="H389" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>salino</t>
         </is>
       </c>
       <c r="I389" t="inlineStr">
@@ -24385,7 +24385,7 @@
       </c>
       <c r="H390" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sarafl</t>
         </is>
       </c>
       <c r="I390" t="inlineStr">
@@ -24691,7 +24691,7 @@
       </c>
       <c r="H395" t="inlineStr">
         <is>
-          <t>siso</t>
+          <t>siso,sisomy</t>
         </is>
       </c>
       <c r="I395" t="inlineStr">
@@ -24751,7 +24751,7 @@
       </c>
       <c r="H396" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sitafl</t>
         </is>
       </c>
       <c r="I396" t="inlineStr">
@@ -24939,7 +24939,7 @@
       </c>
       <c r="H399" t="inlineStr">
         <is>
-          <t>spa,spar</t>
+          <t>spa,spar,sparfl</t>
         </is>
       </c>
       <c r="I399" t="inlineStr">
@@ -25003,7 +25003,7 @@
       </c>
       <c r="H400" t="inlineStr">
         <is>
-          <t>sc,spe,spec,spt</t>
+          <t>sc,spe,spec,spect,spt</t>
         </is>
       </c>
       <c r="I400" t="inlineStr">
@@ -25067,7 +25067,7 @@
       </c>
       <c r="H401" t="inlineStr">
         <is>
-          <t>spir</t>
+          <t>sipram,spir,spiram</t>
         </is>
       </c>
       <c r="I401" t="inlineStr">
@@ -25257,7 +25257,7 @@
       </c>
       <c r="H404" t="inlineStr">
         <is>
-          <t>s,stm,str,stre</t>
+          <t>s,st1000,st2000,stm,str,stre,strept</t>
         </is>
       </c>
       <c r="I404" t="inlineStr">
@@ -25441,7 +25441,7 @@
       </c>
       <c r="H407" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sulbac</t>
         </is>
       </c>
       <c r="I407" t="inlineStr">
@@ -25505,7 +25505,7 @@
       </c>
       <c r="H408" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sulben</t>
         </is>
       </c>
       <c r="I408" t="inlineStr">
@@ -25623,7 +25623,7 @@
       </c>
       <c r="H410" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sulchl</t>
         </is>
       </c>
       <c r="I410" t="inlineStr">
@@ -25685,7 +25685,7 @@
       </c>
       <c r="H411" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>suldia</t>
         </is>
       </c>
       <c r="I411" t="inlineStr">
@@ -25873,7 +25873,7 @@
       </c>
       <c r="H414" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sdimet</t>
         </is>
       </c>
       <c r="I414" t="inlineStr">
@@ -25937,7 +25937,7 @@
       </c>
       <c r="H415" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>suldim</t>
         </is>
       </c>
       <c r="I415" t="inlineStr">
@@ -26323,7 +26323,7 @@
       </c>
       <c r="H421" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sulmet</t>
         </is>
       </c>
       <c r="I421" t="inlineStr">
@@ -26571,7 +26571,7 @@
       </c>
       <c r="H425" t="inlineStr">
         <is>
-          <t>sfmx,sulf</t>
+          <t>sfmx,sulf,sulfam</t>
         </is>
       </c>
       <c r="I425" t="inlineStr">
@@ -27327,7 +27327,7 @@
       </c>
       <c r="H437" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sulthi</t>
         </is>
       </c>
       <c r="I437" t="inlineStr">
@@ -27449,7 +27449,7 @@
       </c>
       <c r="H439" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sulfiz</t>
         </is>
       </c>
       <c r="I439" t="inlineStr">
@@ -27507,7 +27507,7 @@
       </c>
       <c r="H440" t="inlineStr">
         <is>
-          <t>sfna</t>
+          <t>sfna,sulami</t>
         </is>
       </c>
       <c r="I440" t="inlineStr">
@@ -27565,7 +27565,7 @@
       </c>
       <c r="H441" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sulope</t>
         </is>
       </c>
       <c r="I441" t="inlineStr">
@@ -27627,7 +27627,7 @@
       </c>
       <c r="H442" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>sultos</t>
         </is>
       </c>
       <c r="I442" t="inlineStr">
@@ -27871,7 +27871,7 @@
       </c>
       <c r="H446" t="inlineStr">
         <is>
-          <t>tazo</t>
+          <t>tazo,tazoba</t>
         </is>
       </c>
       <c r="I446" t="inlineStr">
@@ -28057,7 +28057,7 @@
       </c>
       <c r="H449" t="inlineStr">
         <is>
-          <t>tec,tei,teic,tp,tpl,tpn</t>
+          <t>tec,tei,teic,teicop,tp,tpl,tpn</t>
         </is>
       </c>
       <c r="I449" t="inlineStr">
@@ -28179,7 +28179,7 @@
       </c>
       <c r="H451" t="inlineStr">
         <is>
-          <t>tela</t>
+          <t>tela,telava</t>
         </is>
       </c>
       <c r="I451" t="inlineStr">
@@ -28241,7 +28241,7 @@
       </c>
       <c r="H452" t="inlineStr">
         <is>
-          <t>teli</t>
+          <t>teli,telith</t>
         </is>
       </c>
       <c r="I452" t="inlineStr">
@@ -28305,7 +28305,7 @@
       </c>
       <c r="H453" t="inlineStr">
         <is>
-          <t>tema</t>
+          <t>tema,temafl</t>
         </is>
       </c>
       <c r="I453" t="inlineStr">
@@ -28369,7 +28369,7 @@
       </c>
       <c r="H454" t="inlineStr">
         <is>
-          <t>temo</t>
+          <t>temo,temoci</t>
         </is>
       </c>
       <c r="I454" t="inlineStr">
@@ -28617,7 +28617,7 @@
       </c>
       <c r="H458" t="inlineStr">
         <is>
-          <t>tc,te,tet,tetr</t>
+          <t>tc,te,tet,tetcyc,tetr,tetra</t>
         </is>
       </c>
       <c r="I458" t="inlineStr">
@@ -28919,7 +28919,7 @@
       </c>
       <c r="H463" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>thiaph</t>
         </is>
       </c>
       <c r="I463" t="inlineStr">
@@ -29105,7 +29105,7 @@
       </c>
       <c r="H466" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>tiamul</t>
         </is>
       </c>
       <c r="I466" t="inlineStr">
@@ -29167,7 +29167,7 @@
       </c>
       <c r="H467" t="inlineStr">
         <is>
-          <t>tc,ti,tic,tica</t>
+          <t>tc,ti,tic,tica,ticarc</t>
         </is>
       </c>
       <c r="I467" t="inlineStr">
@@ -29231,7 +29231,7 @@
       </c>
       <c r="H468" t="inlineStr">
         <is>
-          <t>t/c,tcc,ticl,tim,tlc</t>
+          <t>t/c,tcc,ticcla,ticl,tim,tlc</t>
         </is>
       </c>
       <c r="I468" t="inlineStr">
@@ -29295,7 +29295,7 @@
       </c>
       <c r="H469" t="inlineStr">
         <is>
-          <t>tgc,tig,tige</t>
+          <t>tgc,tig,tige,tigecy</t>
         </is>
       </c>
       <c r="I469" t="inlineStr">
@@ -29529,7 +29529,7 @@
       </c>
       <c r="H473" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>tilmic</t>
         </is>
       </c>
       <c r="I473" t="inlineStr">
@@ -29895,7 +29895,7 @@
       </c>
       <c r="H479" t="inlineStr">
         <is>
-          <t>nn,tm,to,tob,tobr</t>
+          <t>nn,tm,to,tob,tobr,tobram</t>
         </is>
       </c>
       <c r="I479" t="inlineStr">
@@ -30013,7 +30013,7 @@
       </c>
       <c r="H481" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>tosufl</t>
         </is>
       </c>
       <c r="I481" t="inlineStr">
@@ -30143,7 +30143,7 @@
       </c>
       <c r="H483" t="inlineStr">
         <is>
-          <t>cot,cotrim,sxt,t/s,tms,trsu,trsx,ts</t>
+          <t>cot,cotrim,sxt,t/s,tms,trisul,trsu,trsx,ts</t>
         </is>
       </c>
       <c r="I483" t="inlineStr">
@@ -30265,7 +30265,7 @@
       </c>
       <c r="H485" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>trospe</t>
         </is>
       </c>
       <c r="I485" t="inlineStr">
@@ -30327,7 +30327,7 @@
       </c>
       <c r="H486" t="inlineStr">
         <is>
-          <t>trov</t>
+          <t>trov,trovaf</t>
         </is>
       </c>
       <c r="I486" t="inlineStr">
@@ -30389,7 +30389,7 @@
       </c>
       <c r="H487" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>tulath</t>
         </is>
       </c>
       <c r="I487" t="inlineStr">
@@ -30447,7 +30447,7 @@
       </c>
       <c r="H488" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>tylo</t>
         </is>
       </c>
       <c r="I488" t="inlineStr">
@@ -30625,7 +30625,7 @@
       </c>
       <c r="H491" t="inlineStr">
         <is>
-          <t>va,van,vanc</t>
+          <t>va,van,vanc,vancom</t>
         </is>
       </c>
       <c r="I491" t="inlineStr">
@@ -30865,7 +30865,7 @@
       </c>
       <c r="H495" t="inlineStr">
         <is>
-          <t>vori,vrc</t>
+          <t>vori,vorico,vrc</t>
         </is>
       </c>
       <c r="I495" t="inlineStr">

</xml_diff>

<commit_message>
(v3.0.1.9018) fixes #249 updates AB groups
</commit_message>
<xml_diff>
--- a/data-raw/datasets/antimicrobials.xlsx
+++ b/data-raw/datasets/antimicrobials.xlsx
@@ -3147,7 +3147,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Trimethoprims,Sulfonamides</t>
+          <t>Trimethoprims</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -14267,7 +14267,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Trimethoprims</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
@@ -14761,7 +14761,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Antimycobacterials</t>
+          <t>Trimethoprims,Sulfonamides,Antimycobacterials</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
@@ -19869,7 +19869,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Trimethoprims,Sulfonamides</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -25607,7 +25607,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Sulfonamides</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -25791,7 +25791,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>Trimethoprims</t>
+          <t>Trimethoprims,Sulfonamides</t>
         </is>
       </c>
       <c r="E413" t="inlineStr">
@@ -25981,7 +25981,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>Trimethoprims</t>
+          <t>Trimethoprims,Sulfonamides</t>
         </is>
       </c>
       <c r="E416" t="inlineStr">
@@ -26367,7 +26367,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>Trimethoprims</t>
+          <t>Trimethoprims,Sulfonamides</t>
         </is>
       </c>
       <c r="E422" t="inlineStr">
@@ -26429,7 +26429,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Sulfonamides</t>
         </is>
       </c>
       <c r="E423" t="inlineStr">
@@ -26805,7 +26805,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>Trimethoprims</t>
+          <t>Trimethoprims,Sulfonamides</t>
         </is>
       </c>
       <c r="E429" t="inlineStr">
@@ -26933,7 +26933,7 @@
       </c>
       <c r="D431" t="inlineStr">
         <is>
-          <t>Trimethoprims</t>
+          <t>Trimethoprims,Sulfonamides</t>
         </is>
       </c>
       <c r="E431" t="inlineStr">
@@ -27249,7 +27249,7 @@
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Sulfonamides</t>
         </is>
       </c>
       <c r="E436" t="inlineStr">
@@ -27433,7 +27433,7 @@
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Sulfonamides</t>
         </is>
       </c>
       <c r="E439" t="inlineStr">
@@ -27491,7 +27491,7 @@
       </c>
       <c r="D440" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Sulfonamides</t>
         </is>
       </c>
       <c r="E440" t="inlineStr">
@@ -28779,7 +28779,7 @@
       </c>
       <c r="D461" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Tetracyclines</t>
         </is>
       </c>
       <c r="E461" t="inlineStr">
@@ -30181,7 +30181,7 @@
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>Trimethoprims</t>
+          <t>Trimethoprims,Sulfonamides</t>
         </is>
       </c>
       <c r="E484" t="inlineStr">

</xml_diff>